<commit_message>
Add Ward's 400 All 5 Model
</commit_message>
<xml_diff>
--- a/resources/datasets/MigratoryModel/CombinedMigratoryModel_GuthrieZone_Path - AllModels.xlsx
+++ b/resources/datasets/MigratoryModel/CombinedMigratoryModel_GuthrieZone_Path - AllModels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby Ford\Desktop\BantuMigration\Github\Datasets\MigratoryModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby Ford\Desktop\BantuMigration\Github\resources\datasets\MigratoryModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD309C8-1ED0-4987-91B5-2E9BDC010685}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412E6434-33C2-48B8-9CD8-57DC91774D5C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{48220AAF-5FA7-46D3-8056-2130CE6EF7AB}"/>
   </bookViews>
@@ -17,9 +17,9 @@
     <sheet name="ZoneCenterLocations" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MigratoryModel_TableauData!$A$1:$I$291</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MigratoryModel_TableauData!$A$1:$J$381</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1850" uniqueCount="115">
   <si>
     <t>A</t>
   </si>
@@ -290,6 +290,90 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>AMNH - Combined 400 (all 5)</t>
+  </si>
+  <si>
+    <t>C-A</t>
+  </si>
+  <si>
+    <t>B-S</t>
+  </si>
+  <si>
+    <t>S-A</t>
+  </si>
+  <si>
+    <t>A-P</t>
+  </si>
+  <si>
+    <t>S-M</t>
+  </si>
+  <si>
+    <t>M-A</t>
+  </si>
+  <si>
+    <t>A-N</t>
+  </si>
+  <si>
+    <t>A-D</t>
+  </si>
+  <si>
+    <t>D-Y</t>
+  </si>
+  <si>
+    <t>M-B</t>
+  </si>
+  <si>
+    <t>M-C</t>
+  </si>
+  <si>
+    <t>M-K</t>
+  </si>
+  <si>
+    <t>M-Y</t>
+  </si>
+  <si>
+    <t>K-P</t>
+  </si>
+  <si>
+    <t>M-E</t>
+  </si>
+  <si>
+    <t>S-B</t>
+  </si>
+  <si>
+    <t>S-K</t>
+  </si>
+  <si>
+    <t>S-H</t>
+  </si>
+  <si>
+    <t>K-B</t>
+  </si>
+  <si>
+    <t>S-J</t>
+  </si>
+  <si>
+    <t>J-D</t>
+  </si>
+  <si>
+    <t>J-R</t>
+  </si>
+  <si>
+    <t>R-G</t>
+  </si>
+  <si>
+    <t>R-K</t>
+  </si>
+  <si>
+    <t>B-A</t>
+  </si>
+  <si>
+    <t>B-D</t>
+  </si>
+  <si>
+    <t>S-L</t>
   </si>
 </sst>
 </file>
@@ -641,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB7D369B-DF5B-472F-B73D-7CCA41A92755}">
-  <dimension ref="A1:J291"/>
+  <dimension ref="A1:J381"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
+      <selection activeCell="G286" sqref="G286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9733,7 +9817,2618 @@
         <v>1</v>
       </c>
     </row>
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>54</v>
+      </c>
+      <c r="B292">
+        <v>1</v>
+      </c>
+      <c r="C292" t="s">
+        <v>36</v>
+      </c>
+      <c r="D292">
+        <v>2.3488888888888888</v>
+      </c>
+      <c r="E292">
+        <v>10.31111111111111</v>
+      </c>
+      <c r="F292" t="s">
+        <v>0</v>
+      </c>
+      <c r="H292" t="s">
+        <v>87</v>
+      </c>
+      <c r="I292" t="s">
+        <v>79</v>
+      </c>
+      <c r="J292">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>54</v>
+      </c>
+      <c r="B293">
+        <v>2</v>
+      </c>
+      <c r="C293" t="s">
+        <v>36</v>
+      </c>
+      <c r="D293">
+        <v>-0.40769230769230752</v>
+      </c>
+      <c r="E293">
+        <v>21.388461538461538</v>
+      </c>
+      <c r="F293" t="s">
+        <v>2</v>
+      </c>
+      <c r="H293" t="s">
+        <v>87</v>
+      </c>
+      <c r="I293" t="s">
+        <v>79</v>
+      </c>
+      <c r="J293">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>88</v>
+      </c>
+      <c r="B294">
+        <v>1</v>
+      </c>
+      <c r="C294" t="s">
+        <v>36</v>
+      </c>
+      <c r="D294">
+        <v>-0.40769230769230752</v>
+      </c>
+      <c r="E294">
+        <v>21.388461538461538</v>
+      </c>
+      <c r="F294" t="s">
+        <v>2</v>
+      </c>
+      <c r="H294" t="s">
+        <v>87</v>
+      </c>
+      <c r="I294" t="s">
+        <v>79</v>
+      </c>
+      <c r="J294">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>88</v>
+      </c>
+      <c r="B295">
+        <v>2</v>
+      </c>
+      <c r="C295" t="s">
+        <v>36</v>
+      </c>
+      <c r="D295">
+        <v>2.3488888888888888</v>
+      </c>
+      <c r="E295">
+        <v>10.31111111111111</v>
+      </c>
+      <c r="F295" t="s">
+        <v>0</v>
+      </c>
+      <c r="H295" t="s">
+        <v>87</v>
+      </c>
+      <c r="I295" t="s">
+        <v>79</v>
+      </c>
+      <c r="J295">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>18</v>
+      </c>
+      <c r="B296">
+        <v>1</v>
+      </c>
+      <c r="C296" t="s">
+        <v>36</v>
+      </c>
+      <c r="D296">
+        <v>2.3488888888888888</v>
+      </c>
+      <c r="E296">
+        <v>10.31111111111111</v>
+      </c>
+      <c r="F296" t="s">
+        <v>0</v>
+      </c>
+      <c r="H296" t="s">
+        <v>87</v>
+      </c>
+      <c r="I296" t="s">
+        <v>79</v>
+      </c>
+      <c r="J296">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>18</v>
+      </c>
+      <c r="B297">
+        <v>2</v>
+      </c>
+      <c r="C297" t="s">
+        <v>36</v>
+      </c>
+      <c r="D297">
+        <v>-1.753125</v>
+      </c>
+      <c r="E297">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F297" t="s">
+        <v>1</v>
+      </c>
+      <c r="H297" t="s">
+        <v>87</v>
+      </c>
+      <c r="I297" t="s">
+        <v>79</v>
+      </c>
+      <c r="J297">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>88</v>
+      </c>
+      <c r="B298">
+        <v>1</v>
+      </c>
+      <c r="C298" t="s">
+        <v>36</v>
+      </c>
+      <c r="D298">
+        <v>-0.40769230769230752</v>
+      </c>
+      <c r="E298">
+        <v>21.388461538461538</v>
+      </c>
+      <c r="F298" t="s">
+        <v>2</v>
+      </c>
+      <c r="H298" t="s">
+        <v>87</v>
+      </c>
+      <c r="I298" t="s">
+        <v>79</v>
+      </c>
+      <c r="J298">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>88</v>
+      </c>
+      <c r="B299">
+        <v>2</v>
+      </c>
+      <c r="C299" t="s">
+        <v>36</v>
+      </c>
+      <c r="D299">
+        <v>2.3488888888888888</v>
+      </c>
+      <c r="E299">
+        <v>10.31111111111111</v>
+      </c>
+      <c r="F299" t="s">
+        <v>0</v>
+      </c>
+      <c r="H299" t="s">
+        <v>87</v>
+      </c>
+      <c r="I299" t="s">
+        <v>79</v>
+      </c>
+      <c r="J299">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>18</v>
+      </c>
+      <c r="B300">
+        <v>1</v>
+      </c>
+      <c r="C300" t="s">
+        <v>36</v>
+      </c>
+      <c r="D300">
+        <v>2.3488888888888888</v>
+      </c>
+      <c r="E300">
+        <v>10.31111111111111</v>
+      </c>
+      <c r="F300" t="s">
+        <v>0</v>
+      </c>
+      <c r="H300" t="s">
+        <v>87</v>
+      </c>
+      <c r="I300" t="s">
+        <v>79</v>
+      </c>
+      <c r="J300">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>18</v>
+      </c>
+      <c r="B301">
+        <v>2</v>
+      </c>
+      <c r="C301" t="s">
+        <v>36</v>
+      </c>
+      <c r="D301">
+        <v>-1.753125</v>
+      </c>
+      <c r="E301">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F301" t="s">
+        <v>1</v>
+      </c>
+      <c r="H301" t="s">
+        <v>87</v>
+      </c>
+      <c r="I301" t="s">
+        <v>79</v>
+      </c>
+      <c r="J301">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>89</v>
+      </c>
+      <c r="B302">
+        <v>1</v>
+      </c>
+      <c r="C302" t="s">
+        <v>36</v>
+      </c>
+      <c r="D302">
+        <v>-1.753125</v>
+      </c>
+      <c r="E302">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F302" t="s">
+        <v>1</v>
+      </c>
+      <c r="H302" t="s">
+        <v>87</v>
+      </c>
+      <c r="I302" t="s">
+        <v>79</v>
+      </c>
+      <c r="J302">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>89</v>
+      </c>
+      <c r="B303">
+        <v>2</v>
+      </c>
+      <c r="C303" t="s">
+        <v>36</v>
+      </c>
+      <c r="D303">
+        <v>-23.125</v>
+      </c>
+      <c r="E303">
+        <v>29.665624999999999</v>
+      </c>
+      <c r="F303" t="s">
+        <v>15</v>
+      </c>
+      <c r="H303" t="s">
+        <v>87</v>
+      </c>
+      <c r="I303" t="s">
+        <v>79</v>
+      </c>
+      <c r="J303">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>90</v>
+      </c>
+      <c r="B304">
+        <v>1</v>
+      </c>
+      <c r="C304" t="s">
+        <v>36</v>
+      </c>
+      <c r="D304">
+        <v>-23.125</v>
+      </c>
+      <c r="E304">
+        <v>29.665624999999999</v>
+      </c>
+      <c r="F304" t="s">
+        <v>15</v>
+      </c>
+      <c r="H304" t="s">
+        <v>87</v>
+      </c>
+      <c r="I304" t="s">
+        <v>79</v>
+      </c>
+      <c r="J304">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>90</v>
+      </c>
+      <c r="B305">
+        <v>2</v>
+      </c>
+      <c r="C305" t="s">
+        <v>36</v>
+      </c>
+      <c r="D305">
+        <v>2.3488888888888888</v>
+      </c>
+      <c r="E305">
+        <v>10.31111111111111</v>
+      </c>
+      <c r="F305" t="s">
+        <v>0</v>
+      </c>
+      <c r="H305" t="s">
+        <v>87</v>
+      </c>
+      <c r="I305" t="s">
+        <v>79</v>
+      </c>
+      <c r="J305">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>91</v>
+      </c>
+      <c r="B306">
+        <v>1</v>
+      </c>
+      <c r="C306" t="s">
+        <v>36</v>
+      </c>
+      <c r="D306">
+        <v>2.3488888888888888</v>
+      </c>
+      <c r="E306">
+        <v>10.31111111111111</v>
+      </c>
+      <c r="F306" t="s">
+        <v>0</v>
+      </c>
+      <c r="H306" t="s">
+        <v>87</v>
+      </c>
+      <c r="I306" t="s">
+        <v>79</v>
+      </c>
+      <c r="J306">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>91</v>
+      </c>
+      <c r="B307">
+        <v>2</v>
+      </c>
+      <c r="C307" t="s">
+        <v>36</v>
+      </c>
+      <c r="D307">
+        <v>-13.3</v>
+      </c>
+      <c r="E307">
+        <v>39.125</v>
+      </c>
+      <c r="F307" t="s">
+        <v>13</v>
+      </c>
+      <c r="H307" t="s">
+        <v>87</v>
+      </c>
+      <c r="I307" t="s">
+        <v>79</v>
+      </c>
+      <c r="J307">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>92</v>
+      </c>
+      <c r="B308">
+        <v>1</v>
+      </c>
+      <c r="C308" t="s">
+        <v>36</v>
+      </c>
+      <c r="D308">
+        <v>-23.125</v>
+      </c>
+      <c r="E308">
+        <v>29.665624999999999</v>
+      </c>
+      <c r="F308" t="s">
+        <v>15</v>
+      </c>
+      <c r="H308" t="s">
+        <v>87</v>
+      </c>
+      <c r="I308" t="s">
+        <v>79</v>
+      </c>
+      <c r="J308">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>92</v>
+      </c>
+      <c r="B309">
+        <v>2</v>
+      </c>
+      <c r="C309" t="s">
+        <v>36</v>
+      </c>
+      <c r="D309">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E309">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F309" t="s">
+        <v>11</v>
+      </c>
+      <c r="H309" t="s">
+        <v>87</v>
+      </c>
+      <c r="I309" t="s">
+        <v>79</v>
+      </c>
+      <c r="J309">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>93</v>
+      </c>
+      <c r="B310">
+        <v>1</v>
+      </c>
+      <c r="C310" t="s">
+        <v>36</v>
+      </c>
+      <c r="D310">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E310">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F310" t="s">
+        <v>11</v>
+      </c>
+      <c r="H310" t="s">
+        <v>87</v>
+      </c>
+      <c r="I310" t="s">
+        <v>79</v>
+      </c>
+      <c r="J310">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>93</v>
+      </c>
+      <c r="B311">
+        <v>2</v>
+      </c>
+      <c r="C311" t="s">
+        <v>36</v>
+      </c>
+      <c r="D311">
+        <v>2.3488888888888888</v>
+      </c>
+      <c r="E311">
+        <v>10.31111111111111</v>
+      </c>
+      <c r="F311" t="s">
+        <v>0</v>
+      </c>
+      <c r="H311" t="s">
+        <v>87</v>
+      </c>
+      <c r="I311" t="s">
+        <v>79</v>
+      </c>
+      <c r="J311">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>94</v>
+      </c>
+      <c r="B312">
+        <v>1</v>
+      </c>
+      <c r="C312" t="s">
+        <v>36</v>
+      </c>
+      <c r="D312">
+        <v>2.3488888888888888</v>
+      </c>
+      <c r="E312">
+        <v>10.31111111111111</v>
+      </c>
+      <c r="F312" t="s">
+        <v>0</v>
+      </c>
+      <c r="H312" t="s">
+        <v>87</v>
+      </c>
+      <c r="I312" t="s">
+        <v>79</v>
+      </c>
+      <c r="J312">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>94</v>
+      </c>
+      <c r="B313">
+        <v>2</v>
+      </c>
+      <c r="C313" t="s">
+        <v>36</v>
+      </c>
+      <c r="D313">
+        <v>-13.557142857142859</v>
+      </c>
+      <c r="E313">
+        <v>33.514285714285712</v>
+      </c>
+      <c r="F313" t="s">
+        <v>12</v>
+      </c>
+      <c r="H313" t="s">
+        <v>87</v>
+      </c>
+      <c r="I313" t="s">
+        <v>79</v>
+      </c>
+      <c r="J313">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>95</v>
+      </c>
+      <c r="B314">
+        <v>1</v>
+      </c>
+      <c r="C314" t="s">
+        <v>36</v>
+      </c>
+      <c r="D314">
+        <v>2.3488888888888888</v>
+      </c>
+      <c r="E314">
+        <v>10.31111111111111</v>
+      </c>
+      <c r="F314" t="s">
+        <v>0</v>
+      </c>
+      <c r="H314" t="s">
+        <v>87</v>
+      </c>
+      <c r="I314" t="s">
+        <v>79</v>
+      </c>
+      <c r="J314">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>95</v>
+      </c>
+      <c r="B315">
+        <v>2</v>
+      </c>
+      <c r="C315" t="s">
+        <v>36</v>
+      </c>
+      <c r="D315">
+        <v>-1.78</v>
+      </c>
+      <c r="E315">
+        <v>27.603999999999996</v>
+      </c>
+      <c r="F315" t="s">
+        <v>3</v>
+      </c>
+      <c r="H315" t="s">
+        <v>87</v>
+      </c>
+      <c r="I315" t="s">
+        <v>79</v>
+      </c>
+      <c r="J315">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>96</v>
+      </c>
+      <c r="B316">
+        <v>1</v>
+      </c>
+      <c r="C316" t="s">
+        <v>36</v>
+      </c>
+      <c r="D316">
+        <v>-1.78</v>
+      </c>
+      <c r="E316">
+        <v>27.603999999999996</v>
+      </c>
+      <c r="F316" t="s">
+        <v>3</v>
+      </c>
+      <c r="H316" t="s">
+        <v>87</v>
+      </c>
+      <c r="I316" t="s">
+        <v>79</v>
+      </c>
+      <c r="J316">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>23</v>
+      </c>
+      <c r="B317">
+        <v>2</v>
+      </c>
+      <c r="C317" t="s">
+        <v>36</v>
+      </c>
+      <c r="D317">
+        <v>-9.16</v>
+      </c>
+      <c r="E317">
+        <v>26.439999999999998</v>
+      </c>
+      <c r="F317" t="s">
+        <v>10</v>
+      </c>
+      <c r="H317" t="s">
+        <v>87</v>
+      </c>
+      <c r="I317" t="s">
+        <v>79</v>
+      </c>
+      <c r="J317">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>97</v>
+      </c>
+      <c r="B318">
+        <v>1</v>
+      </c>
+      <c r="C318" t="s">
+        <v>35</v>
+      </c>
+      <c r="D318">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E318">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F318" t="s">
+        <v>11</v>
+      </c>
+      <c r="H318" t="s">
+        <v>87</v>
+      </c>
+      <c r="I318" t="s">
+        <v>79</v>
+      </c>
+      <c r="J318">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>97</v>
+      </c>
+      <c r="B319">
+        <v>2</v>
+      </c>
+      <c r="C319" t="s">
+        <v>35</v>
+      </c>
+      <c r="D319">
+        <v>-1.753125</v>
+      </c>
+      <c r="E319">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F319" t="s">
+        <v>1</v>
+      </c>
+      <c r="H319" t="s">
+        <v>87</v>
+      </c>
+      <c r="I319" t="s">
+        <v>79</v>
+      </c>
+      <c r="J319">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>98</v>
+      </c>
+      <c r="B320">
+        <v>1</v>
+      </c>
+      <c r="C320" t="s">
+        <v>35</v>
+      </c>
+      <c r="D320">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E320">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F320" t="s">
+        <v>11</v>
+      </c>
+      <c r="H320" t="s">
+        <v>87</v>
+      </c>
+      <c r="I320" t="s">
+        <v>79</v>
+      </c>
+      <c r="J320">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>98</v>
+      </c>
+      <c r="B321">
+        <v>2</v>
+      </c>
+      <c r="C321" t="s">
+        <v>35</v>
+      </c>
+      <c r="D321">
+        <v>-0.40769230769230752</v>
+      </c>
+      <c r="E321">
+        <v>21.388461538461538</v>
+      </c>
+      <c r="F321" t="s">
+        <v>2</v>
+      </c>
+      <c r="H321" t="s">
+        <v>87</v>
+      </c>
+      <c r="I321" t="s">
+        <v>79</v>
+      </c>
+      <c r="J321">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>99</v>
+      </c>
+      <c r="B322">
+        <v>1</v>
+      </c>
+      <c r="C322" t="s">
+        <v>35</v>
+      </c>
+      <c r="D322">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E322">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F322" t="s">
+        <v>11</v>
+      </c>
+      <c r="H322" t="s">
+        <v>87</v>
+      </c>
+      <c r="I322" t="s">
+        <v>79</v>
+      </c>
+      <c r="J322">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>99</v>
+      </c>
+      <c r="B323">
+        <v>2</v>
+      </c>
+      <c r="C323" t="s">
+        <v>35</v>
+      </c>
+      <c r="D323">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E323">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F323" t="s">
+        <v>9</v>
+      </c>
+      <c r="H323" t="s">
+        <v>87</v>
+      </c>
+      <c r="I323" t="s">
+        <v>79</v>
+      </c>
+      <c r="J323">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>100</v>
+      </c>
+      <c r="B324">
+        <v>1</v>
+      </c>
+      <c r="C324" t="s">
+        <v>35</v>
+      </c>
+      <c r="D324">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E324">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F324" t="s">
+        <v>11</v>
+      </c>
+      <c r="H324" t="s">
+        <v>87</v>
+      </c>
+      <c r="I324" t="s">
+        <v>79</v>
+      </c>
+      <c r="J324">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>53</v>
+      </c>
+      <c r="B325">
+        <v>2</v>
+      </c>
+      <c r="C325" t="s">
+        <v>35</v>
+      </c>
+      <c r="D325">
+        <v>-9.16</v>
+      </c>
+      <c r="E325">
+        <v>26.439999999999998</v>
+      </c>
+      <c r="F325" t="s">
+        <v>10</v>
+      </c>
+      <c r="H325" t="s">
+        <v>87</v>
+      </c>
+      <c r="I325" t="s">
+        <v>79</v>
+      </c>
+      <c r="J325">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>99</v>
+      </c>
+      <c r="B326">
+        <v>1</v>
+      </c>
+      <c r="C326" t="s">
+        <v>35</v>
+      </c>
+      <c r="D326">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E326">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F326" t="s">
+        <v>11</v>
+      </c>
+      <c r="H326" t="s">
+        <v>87</v>
+      </c>
+      <c r="I326" t="s">
+        <v>79</v>
+      </c>
+      <c r="J326">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>99</v>
+      </c>
+      <c r="B327">
+        <v>2</v>
+      </c>
+      <c r="C327" t="s">
+        <v>35</v>
+      </c>
+      <c r="D327">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E327">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F327" t="s">
+        <v>9</v>
+      </c>
+      <c r="H327" t="s">
+        <v>87</v>
+      </c>
+      <c r="I327" t="s">
+        <v>79</v>
+      </c>
+      <c r="J327">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>101</v>
+      </c>
+      <c r="B328">
+        <v>1</v>
+      </c>
+      <c r="C328" t="s">
+        <v>35</v>
+      </c>
+      <c r="D328">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E328">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F328" t="s">
+        <v>9</v>
+      </c>
+      <c r="H328" t="s">
+        <v>87</v>
+      </c>
+      <c r="I328" t="s">
+        <v>79</v>
+      </c>
+      <c r="J328">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>101</v>
+      </c>
+      <c r="B329">
+        <v>2</v>
+      </c>
+      <c r="C329" t="s">
+        <v>35</v>
+      </c>
+      <c r="D329">
+        <v>-13.3</v>
+      </c>
+      <c r="E329">
+        <v>39.125</v>
+      </c>
+      <c r="F329" t="s">
+        <v>13</v>
+      </c>
+      <c r="H329" t="s">
+        <v>87</v>
+      </c>
+      <c r="I329" t="s">
+        <v>79</v>
+      </c>
+      <c r="J329">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>31</v>
+      </c>
+      <c r="B330">
+        <v>1</v>
+      </c>
+      <c r="C330" t="s">
+        <v>35</v>
+      </c>
+      <c r="D330">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E330">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F330" t="s">
+        <v>11</v>
+      </c>
+      <c r="H330" t="s">
+        <v>87</v>
+      </c>
+      <c r="I330" t="s">
+        <v>79</v>
+      </c>
+      <c r="J330">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>31</v>
+      </c>
+      <c r="B331">
+        <v>2</v>
+      </c>
+      <c r="C331" t="s">
+        <v>35</v>
+      </c>
+      <c r="D331">
+        <v>-13.557142857142859</v>
+      </c>
+      <c r="E331">
+        <v>33.514285714285712</v>
+      </c>
+      <c r="F331" t="s">
+        <v>12</v>
+      </c>
+      <c r="H331" t="s">
+        <v>87</v>
+      </c>
+      <c r="I331" t="s">
+        <v>79</v>
+      </c>
+      <c r="J331">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>68</v>
+      </c>
+      <c r="B332">
+        <v>1</v>
+      </c>
+      <c r="C332" t="s">
+        <v>35</v>
+      </c>
+      <c r="D332">
+        <v>-13.557142857142859</v>
+      </c>
+      <c r="E332">
+        <v>33.514285714285712</v>
+      </c>
+      <c r="F332" t="s">
+        <v>12</v>
+      </c>
+      <c r="H332" t="s">
+        <v>87</v>
+      </c>
+      <c r="I332" t="s">
+        <v>79</v>
+      </c>
+      <c r="J332">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>68</v>
+      </c>
+      <c r="B333">
+        <v>2</v>
+      </c>
+      <c r="C333" t="s">
+        <v>35</v>
+      </c>
+      <c r="D333">
+        <v>-23.125</v>
+      </c>
+      <c r="E333">
+        <v>29.665624999999999</v>
+      </c>
+      <c r="F333" t="s">
+        <v>15</v>
+      </c>
+      <c r="H333" t="s">
+        <v>87</v>
+      </c>
+      <c r="I333" t="s">
+        <v>79</v>
+      </c>
+      <c r="J333">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>102</v>
+      </c>
+      <c r="B334">
+        <v>1</v>
+      </c>
+      <c r="C334" t="s">
+        <v>36</v>
+      </c>
+      <c r="D334">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E334">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F334" t="s">
+        <v>11</v>
+      </c>
+      <c r="H334" t="s">
+        <v>87</v>
+      </c>
+      <c r="I334" t="s">
+        <v>79</v>
+      </c>
+      <c r="J334">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>102</v>
+      </c>
+      <c r="B335">
+        <v>2</v>
+      </c>
+      <c r="C335" t="s">
+        <v>36</v>
+      </c>
+      <c r="D335">
+        <v>-2.35</v>
+      </c>
+      <c r="E335">
+        <v>38.449999999999996</v>
+      </c>
+      <c r="F335" t="s">
+        <v>4</v>
+      </c>
+      <c r="H335" t="s">
+        <v>87</v>
+      </c>
+      <c r="I335" t="s">
+        <v>79</v>
+      </c>
+      <c r="J335">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>71</v>
+      </c>
+      <c r="B336">
+        <v>1</v>
+      </c>
+      <c r="C336" t="s">
+        <v>36</v>
+      </c>
+      <c r="D336">
+        <v>-2.35</v>
+      </c>
+      <c r="E336">
+        <v>38.449999999999996</v>
+      </c>
+      <c r="F336" t="s">
+        <v>4</v>
+      </c>
+      <c r="H336" t="s">
+        <v>87</v>
+      </c>
+      <c r="I336" t="s">
+        <v>79</v>
+      </c>
+      <c r="J336">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>71</v>
+      </c>
+      <c r="B337">
+        <v>2</v>
+      </c>
+      <c r="C337" t="s">
+        <v>36</v>
+      </c>
+      <c r="D337">
+        <v>-5.85</v>
+      </c>
+      <c r="E337">
+        <v>37.712499999999999</v>
+      </c>
+      <c r="F337" t="s">
+        <v>6</v>
+      </c>
+      <c r="H337" t="s">
+        <v>87</v>
+      </c>
+      <c r="I337" t="s">
+        <v>79</v>
+      </c>
+      <c r="J337">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>26</v>
+      </c>
+      <c r="B338">
+        <v>1</v>
+      </c>
+      <c r="C338" t="s">
+        <v>35</v>
+      </c>
+      <c r="D338">
+        <v>-5.85</v>
+      </c>
+      <c r="E338">
+        <v>37.712499999999999</v>
+      </c>
+      <c r="F338" t="s">
+        <v>6</v>
+      </c>
+      <c r="H338" t="s">
+        <v>87</v>
+      </c>
+      <c r="I338" t="s">
+        <v>79</v>
+      </c>
+      <c r="J338">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>26</v>
+      </c>
+      <c r="B339">
+        <v>2</v>
+      </c>
+      <c r="C339" t="s">
+        <v>35</v>
+      </c>
+      <c r="D339">
+        <v>-2.35</v>
+      </c>
+      <c r="E339">
+        <v>38.449999999999996</v>
+      </c>
+      <c r="F339" t="s">
+        <v>4</v>
+      </c>
+      <c r="H339" t="s">
+        <v>87</v>
+      </c>
+      <c r="I339" t="s">
+        <v>79</v>
+      </c>
+      <c r="J339">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>71</v>
+      </c>
+      <c r="B340">
+        <v>1</v>
+      </c>
+      <c r="C340" t="s">
+        <v>36</v>
+      </c>
+      <c r="D340">
+        <v>-2.35</v>
+      </c>
+      <c r="E340">
+        <v>38.449999999999996</v>
+      </c>
+      <c r="F340" t="s">
+        <v>4</v>
+      </c>
+      <c r="H340" t="s">
+        <v>87</v>
+      </c>
+      <c r="I340" t="s">
+        <v>79</v>
+      </c>
+      <c r="J340">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>71</v>
+      </c>
+      <c r="B341">
+        <v>2</v>
+      </c>
+      <c r="C341" t="s">
+        <v>36</v>
+      </c>
+      <c r="D341">
+        <v>-5.85</v>
+      </c>
+      <c r="E341">
+        <v>37.712499999999999</v>
+      </c>
+      <c r="F341" t="s">
+        <v>6</v>
+      </c>
+      <c r="H341" t="s">
+        <v>87</v>
+      </c>
+      <c r="I341" t="s">
+        <v>79</v>
+      </c>
+      <c r="J341">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>103</v>
+      </c>
+      <c r="B342">
+        <v>1</v>
+      </c>
+      <c r="C342" t="s">
+        <v>35</v>
+      </c>
+      <c r="D342">
+        <v>-23.125</v>
+      </c>
+      <c r="E342">
+        <v>29.665624999999999</v>
+      </c>
+      <c r="F342" t="s">
+        <v>15</v>
+      </c>
+      <c r="H342" t="s">
+        <v>87</v>
+      </c>
+      <c r="I342" t="s">
+        <v>79</v>
+      </c>
+      <c r="J342">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>103</v>
+      </c>
+      <c r="B343">
+        <v>2</v>
+      </c>
+      <c r="C343" t="s">
+        <v>35</v>
+      </c>
+      <c r="D343">
+        <v>-1.753125</v>
+      </c>
+      <c r="E343">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F343" t="s">
+        <v>1</v>
+      </c>
+      <c r="H343" t="s">
+        <v>87</v>
+      </c>
+      <c r="I343" t="s">
+        <v>79</v>
+      </c>
+      <c r="J343">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>114</v>
+      </c>
+      <c r="B344">
+        <v>1</v>
+      </c>
+      <c r="C344" t="s">
+        <v>35</v>
+      </c>
+      <c r="D344">
+        <v>-23.125</v>
+      </c>
+      <c r="E344">
+        <v>29.665624999999999</v>
+      </c>
+      <c r="F344" t="s">
+        <v>15</v>
+      </c>
+      <c r="H344" t="s">
+        <v>87</v>
+      </c>
+      <c r="I344" t="s">
+        <v>79</v>
+      </c>
+      <c r="J344">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>114</v>
+      </c>
+      <c r="B345">
+        <v>2</v>
+      </c>
+      <c r="C345" t="s">
+        <v>35</v>
+      </c>
+      <c r="D345">
+        <v>-9.16</v>
+      </c>
+      <c r="E345">
+        <v>26.439999999999998</v>
+      </c>
+      <c r="F345" t="s">
+        <v>10</v>
+      </c>
+      <c r="H345" t="s">
+        <v>87</v>
+      </c>
+      <c r="I345" t="s">
+        <v>79</v>
+      </c>
+      <c r="J345">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>103</v>
+      </c>
+      <c r="B346">
+        <v>1</v>
+      </c>
+      <c r="C346" t="s">
+        <v>35</v>
+      </c>
+      <c r="D346">
+        <v>-23.125</v>
+      </c>
+      <c r="E346">
+        <v>29.665624999999999</v>
+      </c>
+      <c r="F346" t="s">
+        <v>15</v>
+      </c>
+      <c r="H346" t="s">
+        <v>87</v>
+      </c>
+      <c r="I346" t="s">
+        <v>79</v>
+      </c>
+      <c r="J346">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>103</v>
+      </c>
+      <c r="B347">
+        <v>2</v>
+      </c>
+      <c r="C347" t="s">
+        <v>35</v>
+      </c>
+      <c r="D347">
+        <v>-1.753125</v>
+      </c>
+      <c r="E347">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F347" t="s">
+        <v>1</v>
+      </c>
+      <c r="H347" t="s">
+        <v>87</v>
+      </c>
+      <c r="I347" t="s">
+        <v>79</v>
+      </c>
+      <c r="J347">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>104</v>
+      </c>
+      <c r="B348">
+        <v>1</v>
+      </c>
+      <c r="C348" t="s">
+        <v>35</v>
+      </c>
+      <c r="D348">
+        <v>-23.125</v>
+      </c>
+      <c r="E348">
+        <v>29.665624999999999</v>
+      </c>
+      <c r="F348" t="s">
+        <v>15</v>
+      </c>
+      <c r="H348" t="s">
+        <v>87</v>
+      </c>
+      <c r="I348" t="s">
+        <v>79</v>
+      </c>
+      <c r="J348">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>104</v>
+      </c>
+      <c r="B349">
+        <v>2</v>
+      </c>
+      <c r="C349" t="s">
+        <v>35</v>
+      </c>
+      <c r="D349">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E349">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F349" t="s">
+        <v>9</v>
+      </c>
+      <c r="H349" t="s">
+        <v>87</v>
+      </c>
+      <c r="I349" t="s">
+        <v>79</v>
+      </c>
+      <c r="J349">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>103</v>
+      </c>
+      <c r="B350">
+        <v>1</v>
+      </c>
+      <c r="C350" t="s">
+        <v>35</v>
+      </c>
+      <c r="D350">
+        <v>-23.125</v>
+      </c>
+      <c r="E350">
+        <v>29.665624999999999</v>
+      </c>
+      <c r="F350" t="s">
+        <v>15</v>
+      </c>
+      <c r="H350" t="s">
+        <v>87</v>
+      </c>
+      <c r="I350" t="s">
+        <v>79</v>
+      </c>
+      <c r="J350">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>103</v>
+      </c>
+      <c r="B351">
+        <v>2</v>
+      </c>
+      <c r="C351" t="s">
+        <v>35</v>
+      </c>
+      <c r="D351">
+        <v>-1.753125</v>
+      </c>
+      <c r="E351">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F351" t="s">
+        <v>1</v>
+      </c>
+      <c r="H351" t="s">
+        <v>87</v>
+      </c>
+      <c r="I351" t="s">
+        <v>79</v>
+      </c>
+      <c r="J351">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>105</v>
+      </c>
+      <c r="B352">
+        <v>1</v>
+      </c>
+      <c r="C352" t="s">
+        <v>35</v>
+      </c>
+      <c r="D352">
+        <v>-23.125</v>
+      </c>
+      <c r="E352">
+        <v>29.665624999999999</v>
+      </c>
+      <c r="F352" t="s">
+        <v>15</v>
+      </c>
+      <c r="H352" t="s">
+        <v>87</v>
+      </c>
+      <c r="I352" t="s">
+        <v>79</v>
+      </c>
+      <c r="J352">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>105</v>
+      </c>
+      <c r="B353">
+        <v>2</v>
+      </c>
+      <c r="C353" t="s">
+        <v>35</v>
+      </c>
+      <c r="D353">
+        <v>-5.5714285714285703</v>
+      </c>
+      <c r="E353">
+        <v>15.75</v>
+      </c>
+      <c r="F353" t="s">
+        <v>7</v>
+      </c>
+      <c r="H353" t="s">
+        <v>87</v>
+      </c>
+      <c r="I353" t="s">
+        <v>79</v>
+      </c>
+      <c r="J353">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>104</v>
+      </c>
+      <c r="B354">
+        <v>1</v>
+      </c>
+      <c r="C354" t="s">
+        <v>35</v>
+      </c>
+      <c r="D354">
+        <v>-23.125</v>
+      </c>
+      <c r="E354">
+        <v>29.665624999999999</v>
+      </c>
+      <c r="F354" t="s">
+        <v>15</v>
+      </c>
+      <c r="H354" t="s">
+        <v>87</v>
+      </c>
+      <c r="I354" t="s">
+        <v>79</v>
+      </c>
+      <c r="J354">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>104</v>
+      </c>
+      <c r="B355">
+        <v>2</v>
+      </c>
+      <c r="C355" t="s">
+        <v>35</v>
+      </c>
+      <c r="D355">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E355">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F355" t="s">
+        <v>9</v>
+      </c>
+      <c r="H355" t="s">
+        <v>87</v>
+      </c>
+      <c r="I355" t="s">
+        <v>79</v>
+      </c>
+      <c r="J355">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>106</v>
+      </c>
+      <c r="B356">
+        <v>1</v>
+      </c>
+      <c r="C356" t="s">
+        <v>35</v>
+      </c>
+      <c r="D356">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E356">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F356" t="s">
+        <v>9</v>
+      </c>
+      <c r="H356" t="s">
+        <v>87</v>
+      </c>
+      <c r="I356" t="s">
+        <v>79</v>
+      </c>
+      <c r="J356">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>106</v>
+      </c>
+      <c r="B357">
+        <v>2</v>
+      </c>
+      <c r="C357" t="s">
+        <v>35</v>
+      </c>
+      <c r="D357">
+        <v>-1.753125</v>
+      </c>
+      <c r="E357">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F357" t="s">
+        <v>1</v>
+      </c>
+      <c r="H357" t="s">
+        <v>87</v>
+      </c>
+      <c r="I357" t="s">
+        <v>79</v>
+      </c>
+      <c r="J357">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="358" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>107</v>
+      </c>
+      <c r="B358">
+        <v>1</v>
+      </c>
+      <c r="C358" t="s">
+        <v>36</v>
+      </c>
+      <c r="D358">
+        <v>-23.125</v>
+      </c>
+      <c r="E358">
+        <v>29.665624999999999</v>
+      </c>
+      <c r="F358" t="s">
+        <v>15</v>
+      </c>
+      <c r="H358" t="s">
+        <v>87</v>
+      </c>
+      <c r="I358" t="s">
+        <v>79</v>
+      </c>
+      <c r="J358">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>107</v>
+      </c>
+      <c r="B359">
+        <v>2</v>
+      </c>
+      <c r="C359" t="s">
+        <v>36</v>
+      </c>
+      <c r="D359">
+        <v>-1.44444444444444</v>
+      </c>
+      <c r="E359">
+        <v>30.911111111111115</v>
+      </c>
+      <c r="F359" t="s">
+        <v>8</v>
+      </c>
+      <c r="H359" t="s">
+        <v>87</v>
+      </c>
+      <c r="I359" t="s">
+        <v>79</v>
+      </c>
+      <c r="J359">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>108</v>
+      </c>
+      <c r="B360">
+        <v>1</v>
+      </c>
+      <c r="C360" t="s">
+        <v>35</v>
+      </c>
+      <c r="D360">
+        <v>-1.44444444444444</v>
+      </c>
+      <c r="E360">
+        <v>30.911111111111115</v>
+      </c>
+      <c r="F360" t="s">
+        <v>8</v>
+      </c>
+      <c r="H360" t="s">
+        <v>87</v>
+      </c>
+      <c r="I360" t="s">
+        <v>79</v>
+      </c>
+      <c r="J360">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>108</v>
+      </c>
+      <c r="B361">
+        <v>2</v>
+      </c>
+      <c r="C361" t="s">
+        <v>35</v>
+      </c>
+      <c r="D361">
+        <v>-1.78</v>
+      </c>
+      <c r="E361">
+        <v>27.603999999999996</v>
+      </c>
+      <c r="F361" t="s">
+        <v>3</v>
+      </c>
+      <c r="H361" t="s">
+        <v>87</v>
+      </c>
+      <c r="I361" t="s">
+        <v>79</v>
+      </c>
+      <c r="J361">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>24</v>
+      </c>
+      <c r="B362">
+        <v>1</v>
+      </c>
+      <c r="C362" t="s">
+        <v>35</v>
+      </c>
+      <c r="D362">
+        <v>-1.44444444444444</v>
+      </c>
+      <c r="E362">
+        <v>30.911111111111115</v>
+      </c>
+      <c r="F362" t="s">
+        <v>8</v>
+      </c>
+      <c r="H362" t="s">
+        <v>87</v>
+      </c>
+      <c r="I362" t="s">
+        <v>79</v>
+      </c>
+      <c r="J362">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>24</v>
+      </c>
+      <c r="B363">
+        <v>2</v>
+      </c>
+      <c r="C363" t="s">
+        <v>35</v>
+      </c>
+      <c r="D363">
+        <v>-3.7333333333333329</v>
+      </c>
+      <c r="E363">
+        <v>33</v>
+      </c>
+      <c r="F363" t="s">
+        <v>5</v>
+      </c>
+      <c r="H363" t="s">
+        <v>87</v>
+      </c>
+      <c r="I363" t="s">
+        <v>79</v>
+      </c>
+      <c r="J363">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>109</v>
+      </c>
+      <c r="B364">
+        <v>1</v>
+      </c>
+      <c r="C364" t="s">
+        <v>35</v>
+      </c>
+      <c r="D364">
+        <v>-1.44444444444444</v>
+      </c>
+      <c r="E364">
+        <v>30.911111111111115</v>
+      </c>
+      <c r="F364" t="s">
+        <v>8</v>
+      </c>
+      <c r="H364" t="s">
+        <v>87</v>
+      </c>
+      <c r="I364" t="s">
+        <v>79</v>
+      </c>
+      <c r="J364">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>109</v>
+      </c>
+      <c r="B365">
+        <v>2</v>
+      </c>
+      <c r="C365" t="s">
+        <v>35</v>
+      </c>
+      <c r="D365">
+        <v>-15.824999999999999</v>
+      </c>
+      <c r="E365">
+        <v>15.45</v>
+      </c>
+      <c r="F365" t="s">
+        <v>14</v>
+      </c>
+      <c r="H365" t="s">
+        <v>87</v>
+      </c>
+      <c r="I365" t="s">
+        <v>79</v>
+      </c>
+      <c r="J365">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>110</v>
+      </c>
+      <c r="B366">
+        <v>1</v>
+      </c>
+      <c r="C366" t="s">
+        <v>35</v>
+      </c>
+      <c r="D366">
+        <v>-15.824999999999999</v>
+      </c>
+      <c r="E366">
+        <v>15.45</v>
+      </c>
+      <c r="F366" t="s">
+        <v>14</v>
+      </c>
+      <c r="H366" t="s">
+        <v>87</v>
+      </c>
+      <c r="I366" t="s">
+        <v>79</v>
+      </c>
+      <c r="J366">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>110</v>
+      </c>
+      <c r="B367">
+        <v>2</v>
+      </c>
+      <c r="C367" t="s">
+        <v>35</v>
+      </c>
+      <c r="D367">
+        <v>-5.85</v>
+      </c>
+      <c r="E367">
+        <v>37.712499999999999</v>
+      </c>
+      <c r="F367" t="s">
+        <v>6</v>
+      </c>
+      <c r="H367" t="s">
+        <v>87</v>
+      </c>
+      <c r="I367" t="s">
+        <v>79</v>
+      </c>
+      <c r="J367">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>111</v>
+      </c>
+      <c r="B368">
+        <v>1</v>
+      </c>
+      <c r="C368" t="s">
+        <v>35</v>
+      </c>
+      <c r="D368">
+        <v>-15.824999999999999</v>
+      </c>
+      <c r="E368">
+        <v>15.45</v>
+      </c>
+      <c r="F368" t="s">
+        <v>14</v>
+      </c>
+      <c r="H368" t="s">
+        <v>87</v>
+      </c>
+      <c r="I368" t="s">
+        <v>79</v>
+      </c>
+      <c r="J368">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>111</v>
+      </c>
+      <c r="B369">
+        <v>2</v>
+      </c>
+      <c r="C369" t="s">
+        <v>35</v>
+      </c>
+      <c r="D369">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E369">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F369" t="s">
+        <v>9</v>
+      </c>
+      <c r="H369" t="s">
+        <v>87</v>
+      </c>
+      <c r="I369" t="s">
+        <v>79</v>
+      </c>
+      <c r="J369">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>103</v>
+      </c>
+      <c r="B370">
+        <v>1</v>
+      </c>
+      <c r="C370" t="s">
+        <v>36</v>
+      </c>
+      <c r="D370">
+        <v>-23.125</v>
+      </c>
+      <c r="E370">
+        <v>29.665624999999999</v>
+      </c>
+      <c r="F370" t="s">
+        <v>15</v>
+      </c>
+      <c r="H370" t="s">
+        <v>87</v>
+      </c>
+      <c r="I370" t="s">
+        <v>79</v>
+      </c>
+      <c r="J370">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="371" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>103</v>
+      </c>
+      <c r="B371">
+        <v>2</v>
+      </c>
+      <c r="C371" t="s">
+        <v>36</v>
+      </c>
+      <c r="D371">
+        <v>-1.753125</v>
+      </c>
+      <c r="E371">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F371" t="s">
+        <v>1</v>
+      </c>
+      <c r="H371" t="s">
+        <v>87</v>
+      </c>
+      <c r="I371" t="s">
+        <v>79</v>
+      </c>
+      <c r="J371">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="372" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>112</v>
+      </c>
+      <c r="B372">
+        <v>1</v>
+      </c>
+      <c r="C372" t="s">
+        <v>35</v>
+      </c>
+      <c r="D372">
+        <v>-1.753125</v>
+      </c>
+      <c r="E372">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F372" t="s">
+        <v>1</v>
+      </c>
+      <c r="H372" t="s">
+        <v>87</v>
+      </c>
+      <c r="I372" t="s">
+        <v>79</v>
+      </c>
+      <c r="J372">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>112</v>
+      </c>
+      <c r="B373">
+        <v>2</v>
+      </c>
+      <c r="C373" t="s">
+        <v>35</v>
+      </c>
+      <c r="D373">
+        <v>2.3488888888888888</v>
+      </c>
+      <c r="E373">
+        <v>10.31111111111111</v>
+      </c>
+      <c r="F373" t="s">
+        <v>0</v>
+      </c>
+      <c r="H373" t="s">
+        <v>87</v>
+      </c>
+      <c r="I373" t="s">
+        <v>79</v>
+      </c>
+      <c r="J373">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="374" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>44</v>
+      </c>
+      <c r="B374">
+        <v>1</v>
+      </c>
+      <c r="C374" t="s">
+        <v>35</v>
+      </c>
+      <c r="D374">
+        <v>-1.753125</v>
+      </c>
+      <c r="E374">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F374" t="s">
+        <v>1</v>
+      </c>
+      <c r="H374" t="s">
+        <v>87</v>
+      </c>
+      <c r="I374" t="s">
+        <v>79</v>
+      </c>
+      <c r="J374">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>44</v>
+      </c>
+      <c r="B375">
+        <v>2</v>
+      </c>
+      <c r="C375" t="s">
+        <v>35</v>
+      </c>
+      <c r="D375">
+        <v>-0.40769230769230752</v>
+      </c>
+      <c r="E375">
+        <v>21.388461538461538</v>
+      </c>
+      <c r="F375" t="s">
+        <v>2</v>
+      </c>
+      <c r="H375" t="s">
+        <v>87</v>
+      </c>
+      <c r="I375" t="s">
+        <v>79</v>
+      </c>
+      <c r="J375">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>19</v>
+      </c>
+      <c r="B376">
+        <v>1</v>
+      </c>
+      <c r="C376" t="s">
+        <v>35</v>
+      </c>
+      <c r="D376">
+        <v>-1.753125</v>
+      </c>
+      <c r="E376">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F376" t="s">
+        <v>1</v>
+      </c>
+      <c r="H376" t="s">
+        <v>87</v>
+      </c>
+      <c r="I376" t="s">
+        <v>79</v>
+      </c>
+      <c r="J376">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="377" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>19</v>
+      </c>
+      <c r="B377">
+        <v>2</v>
+      </c>
+      <c r="C377" t="s">
+        <v>35</v>
+      </c>
+      <c r="D377">
+        <v>-5.5714285714285703</v>
+      </c>
+      <c r="E377">
+        <v>15.75</v>
+      </c>
+      <c r="F377" t="s">
+        <v>7</v>
+      </c>
+      <c r="H377" t="s">
+        <v>87</v>
+      </c>
+      <c r="I377" t="s">
+        <v>79</v>
+      </c>
+      <c r="J377">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="378" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>112</v>
+      </c>
+      <c r="B378">
+        <v>1</v>
+      </c>
+      <c r="C378" t="s">
+        <v>35</v>
+      </c>
+      <c r="D378">
+        <v>-1.753125</v>
+      </c>
+      <c r="E378">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F378" t="s">
+        <v>1</v>
+      </c>
+      <c r="H378" t="s">
+        <v>87</v>
+      </c>
+      <c r="I378" t="s">
+        <v>79</v>
+      </c>
+      <c r="J378">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="379" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>112</v>
+      </c>
+      <c r="B379">
+        <v>2</v>
+      </c>
+      <c r="C379" t="s">
+        <v>35</v>
+      </c>
+      <c r="D379">
+        <v>2.3488888888888888</v>
+      </c>
+      <c r="E379">
+        <v>10.31111111111111</v>
+      </c>
+      <c r="F379" t="s">
+        <v>0</v>
+      </c>
+      <c r="H379" t="s">
+        <v>87</v>
+      </c>
+      <c r="I379" t="s">
+        <v>79</v>
+      </c>
+      <c r="J379">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="380" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>113</v>
+      </c>
+      <c r="B380">
+        <v>1</v>
+      </c>
+      <c r="C380" t="s">
+        <v>35</v>
+      </c>
+      <c r="D380">
+        <v>-1.753125</v>
+      </c>
+      <c r="E380">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F380" t="s">
+        <v>1</v>
+      </c>
+      <c r="H380" t="s">
+        <v>87</v>
+      </c>
+      <c r="I380" t="s">
+        <v>79</v>
+      </c>
+      <c r="J380">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>113</v>
+      </c>
+      <c r="B381">
+        <v>2</v>
+      </c>
+      <c r="C381" t="s">
+        <v>35</v>
+      </c>
+      <c r="D381">
+        <v>-1.78</v>
+      </c>
+      <c r="E381">
+        <v>27.603999999999996</v>
+      </c>
+      <c r="F381" t="s">
+        <v>3</v>
+      </c>
+      <c r="H381" t="s">
+        <v>87</v>
+      </c>
+      <c r="I381" t="s">
+        <v>79</v>
+      </c>
+      <c r="J381">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:J381" xr:uid="{303E4824-0DA0-4156-A165-CC92066081A2}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add Jan-2019, AMNH Run
</commit_message>
<xml_diff>
--- a/resources/datasets/MigratoryModel/CombinedMigratoryModel_GuthrieZone_Path - AllModels.xlsx
+++ b/resources/datasets/MigratoryModel/CombinedMigratoryModel_GuthrieZone_Path - AllModels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby Ford\Desktop\BantuMigration\Github\resources\datasets\MigratoryModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412E6434-33C2-48B8-9CD8-57DC91774D5C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771C601A-7E53-4173-B214-E2DC6BB18105}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{48220AAF-5FA7-46D3-8056-2130CE6EF7AB}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1850" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2000" uniqueCount="116">
   <si>
     <t>A</t>
   </si>
@@ -374,6 +374,9 @@
   </si>
   <si>
     <t>S-L</t>
+  </si>
+  <si>
+    <t>AMNH - Combined 400 (all 5) - H</t>
   </si>
 </sst>
 </file>
@@ -725,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB7D369B-DF5B-472F-B73D-7CCA41A92755}">
-  <dimension ref="A1:J381"/>
+  <dimension ref="A1:J411"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
-      <selection activeCell="G286" sqref="G286"/>
+    <sheetView tabSelected="1" topLeftCell="A350" workbookViewId="0">
+      <selection activeCell="L383" sqref="L383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9843,7 +9846,7 @@
         <v>79</v>
       </c>
       <c r="J292">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="293" spans="1:10" x14ac:dyDescent="0.25">
@@ -9872,7 +9875,7 @@
         <v>79</v>
       </c>
       <c r="J293">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="294" spans="1:10" x14ac:dyDescent="0.25">
@@ -9901,7 +9904,7 @@
         <v>79</v>
       </c>
       <c r="J294">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="295" spans="1:10" x14ac:dyDescent="0.25">
@@ -9930,7 +9933,7 @@
         <v>79</v>
       </c>
       <c r="J295">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.25">
@@ -9959,7 +9962,7 @@
         <v>79</v>
       </c>
       <c r="J296">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="297" spans="1:10" x14ac:dyDescent="0.25">
@@ -9988,7 +9991,7 @@
         <v>79</v>
       </c>
       <c r="J297">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="298" spans="1:10" x14ac:dyDescent="0.25">
@@ -10017,7 +10020,7 @@
         <v>79</v>
       </c>
       <c r="J298">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="299" spans="1:10" x14ac:dyDescent="0.25">
@@ -10046,7 +10049,7 @@
         <v>79</v>
       </c>
       <c r="J299">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="300" spans="1:10" x14ac:dyDescent="0.25">
@@ -10075,7 +10078,7 @@
         <v>79</v>
       </c>
       <c r="J300">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.25">
@@ -10104,7 +10107,7 @@
         <v>79</v>
       </c>
       <c r="J301">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.25">
@@ -10133,7 +10136,7 @@
         <v>79</v>
       </c>
       <c r="J302">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="303" spans="1:10" x14ac:dyDescent="0.25">
@@ -10162,7 +10165,7 @@
         <v>79</v>
       </c>
       <c r="J303">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="304" spans="1:10" x14ac:dyDescent="0.25">
@@ -10191,7 +10194,7 @@
         <v>79</v>
       </c>
       <c r="J304">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="305" spans="1:10" x14ac:dyDescent="0.25">
@@ -10220,7 +10223,7 @@
         <v>79</v>
       </c>
       <c r="J305">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="306" spans="1:10" x14ac:dyDescent="0.25">
@@ -10249,7 +10252,7 @@
         <v>79</v>
       </c>
       <c r="J306">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="307" spans="1:10" x14ac:dyDescent="0.25">
@@ -10278,7 +10281,7 @@
         <v>79</v>
       </c>
       <c r="J307">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="308" spans="1:10" x14ac:dyDescent="0.25">
@@ -10307,7 +10310,7 @@
         <v>79</v>
       </c>
       <c r="J308">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="309" spans="1:10" x14ac:dyDescent="0.25">
@@ -10336,7 +10339,7 @@
         <v>79</v>
       </c>
       <c r="J309">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="310" spans="1:10" x14ac:dyDescent="0.25">
@@ -10365,7 +10368,7 @@
         <v>79</v>
       </c>
       <c r="J310">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="311" spans="1:10" x14ac:dyDescent="0.25">
@@ -10394,7 +10397,7 @@
         <v>79</v>
       </c>
       <c r="J311">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="312" spans="1:10" x14ac:dyDescent="0.25">
@@ -10423,7 +10426,7 @@
         <v>79</v>
       </c>
       <c r="J312">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="313" spans="1:10" x14ac:dyDescent="0.25">
@@ -10452,7 +10455,7 @@
         <v>79</v>
       </c>
       <c r="J313">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="314" spans="1:10" x14ac:dyDescent="0.25">
@@ -10481,7 +10484,7 @@
         <v>79</v>
       </c>
       <c r="J314">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="315" spans="1:10" x14ac:dyDescent="0.25">
@@ -10510,7 +10513,7 @@
         <v>79</v>
       </c>
       <c r="J315">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="316" spans="1:10" x14ac:dyDescent="0.25">
@@ -10539,7 +10542,7 @@
         <v>79</v>
       </c>
       <c r="J316">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="317" spans="1:10" x14ac:dyDescent="0.25">
@@ -10568,7 +10571,7 @@
         <v>79</v>
       </c>
       <c r="J317">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="318" spans="1:10" x14ac:dyDescent="0.25">
@@ -10597,7 +10600,7 @@
         <v>79</v>
       </c>
       <c r="J318">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="319" spans="1:10" x14ac:dyDescent="0.25">
@@ -10626,7 +10629,7 @@
         <v>79</v>
       </c>
       <c r="J319">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="320" spans="1:10" x14ac:dyDescent="0.25">
@@ -10655,7 +10658,7 @@
         <v>79</v>
       </c>
       <c r="J320">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="321" spans="1:10" x14ac:dyDescent="0.25">
@@ -10684,7 +10687,7 @@
         <v>79</v>
       </c>
       <c r="J321">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="322" spans="1:10" x14ac:dyDescent="0.25">
@@ -10713,7 +10716,7 @@
         <v>79</v>
       </c>
       <c r="J322">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="323" spans="1:10" x14ac:dyDescent="0.25">
@@ -10742,7 +10745,7 @@
         <v>79</v>
       </c>
       <c r="J323">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="324" spans="1:10" x14ac:dyDescent="0.25">
@@ -10771,7 +10774,7 @@
         <v>79</v>
       </c>
       <c r="J324">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="325" spans="1:10" x14ac:dyDescent="0.25">
@@ -10800,7 +10803,7 @@
         <v>79</v>
       </c>
       <c r="J325">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="326" spans="1:10" x14ac:dyDescent="0.25">
@@ -10829,7 +10832,7 @@
         <v>79</v>
       </c>
       <c r="J326">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="327" spans="1:10" x14ac:dyDescent="0.25">
@@ -10858,7 +10861,7 @@
         <v>79</v>
       </c>
       <c r="J327">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="328" spans="1:10" x14ac:dyDescent="0.25">
@@ -10887,7 +10890,7 @@
         <v>79</v>
       </c>
       <c r="J328">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="329" spans="1:10" x14ac:dyDescent="0.25">
@@ -10916,7 +10919,7 @@
         <v>79</v>
       </c>
       <c r="J329">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="330" spans="1:10" x14ac:dyDescent="0.25">
@@ -10945,7 +10948,7 @@
         <v>79</v>
       </c>
       <c r="J330">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="331" spans="1:10" x14ac:dyDescent="0.25">
@@ -10974,7 +10977,7 @@
         <v>79</v>
       </c>
       <c r="J331">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="332" spans="1:10" x14ac:dyDescent="0.25">
@@ -11003,7 +11006,7 @@
         <v>79</v>
       </c>
       <c r="J332">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="333" spans="1:10" x14ac:dyDescent="0.25">
@@ -11032,7 +11035,7 @@
         <v>79</v>
       </c>
       <c r="J333">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="334" spans="1:10" x14ac:dyDescent="0.25">
@@ -11061,7 +11064,7 @@
         <v>79</v>
       </c>
       <c r="J334">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="335" spans="1:10" x14ac:dyDescent="0.25">
@@ -11090,7 +11093,7 @@
         <v>79</v>
       </c>
       <c r="J335">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="336" spans="1:10" x14ac:dyDescent="0.25">
@@ -11119,7 +11122,7 @@
         <v>79</v>
       </c>
       <c r="J336">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="337" spans="1:10" x14ac:dyDescent="0.25">
@@ -11148,7 +11151,7 @@
         <v>79</v>
       </c>
       <c r="J337">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="338" spans="1:10" x14ac:dyDescent="0.25">
@@ -11177,7 +11180,7 @@
         <v>79</v>
       </c>
       <c r="J338">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="339" spans="1:10" x14ac:dyDescent="0.25">
@@ -11206,7 +11209,7 @@
         <v>79</v>
       </c>
       <c r="J339">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="340" spans="1:10" x14ac:dyDescent="0.25">
@@ -11235,7 +11238,7 @@
         <v>79</v>
       </c>
       <c r="J340">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="341" spans="1:10" x14ac:dyDescent="0.25">
@@ -11264,7 +11267,7 @@
         <v>79</v>
       </c>
       <c r="J341">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="342" spans="1:10" x14ac:dyDescent="0.25">
@@ -11293,7 +11296,7 @@
         <v>79</v>
       </c>
       <c r="J342">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="343" spans="1:10" x14ac:dyDescent="0.25">
@@ -11322,7 +11325,7 @@
         <v>79</v>
       </c>
       <c r="J343">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="344" spans="1:10" x14ac:dyDescent="0.25">
@@ -11351,7 +11354,7 @@
         <v>79</v>
       </c>
       <c r="J344">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="345" spans="1:10" x14ac:dyDescent="0.25">
@@ -11380,7 +11383,7 @@
         <v>79</v>
       </c>
       <c r="J345">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="346" spans="1:10" x14ac:dyDescent="0.25">
@@ -11409,7 +11412,7 @@
         <v>79</v>
       </c>
       <c r="J346">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="347" spans="1:10" x14ac:dyDescent="0.25">
@@ -11438,7 +11441,7 @@
         <v>79</v>
       </c>
       <c r="J347">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="348" spans="1:10" x14ac:dyDescent="0.25">
@@ -11467,7 +11470,7 @@
         <v>79</v>
       </c>
       <c r="J348">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="349" spans="1:10" x14ac:dyDescent="0.25">
@@ -11496,7 +11499,7 @@
         <v>79</v>
       </c>
       <c r="J349">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="350" spans="1:10" x14ac:dyDescent="0.25">
@@ -11525,7 +11528,7 @@
         <v>79</v>
       </c>
       <c r="J350">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="351" spans="1:10" x14ac:dyDescent="0.25">
@@ -11554,7 +11557,7 @@
         <v>79</v>
       </c>
       <c r="J351">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="352" spans="1:10" x14ac:dyDescent="0.25">
@@ -11583,7 +11586,7 @@
         <v>79</v>
       </c>
       <c r="J352">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="353" spans="1:10" x14ac:dyDescent="0.25">
@@ -11612,7 +11615,7 @@
         <v>79</v>
       </c>
       <c r="J353">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="354" spans="1:10" x14ac:dyDescent="0.25">
@@ -11641,7 +11644,7 @@
         <v>79</v>
       </c>
       <c r="J354">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="355" spans="1:10" x14ac:dyDescent="0.25">
@@ -11670,7 +11673,7 @@
         <v>79</v>
       </c>
       <c r="J355">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="356" spans="1:10" x14ac:dyDescent="0.25">
@@ -11699,7 +11702,7 @@
         <v>79</v>
       </c>
       <c r="J356">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="357" spans="1:10" x14ac:dyDescent="0.25">
@@ -11728,7 +11731,7 @@
         <v>79</v>
       </c>
       <c r="J357">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="358" spans="1:10" x14ac:dyDescent="0.25">
@@ -11757,7 +11760,7 @@
         <v>79</v>
       </c>
       <c r="J358">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="359" spans="1:10" x14ac:dyDescent="0.25">
@@ -11786,7 +11789,7 @@
         <v>79</v>
       </c>
       <c r="J359">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="360" spans="1:10" x14ac:dyDescent="0.25">
@@ -11815,7 +11818,7 @@
         <v>79</v>
       </c>
       <c r="J360">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="361" spans="1:10" x14ac:dyDescent="0.25">
@@ -11844,7 +11847,7 @@
         <v>79</v>
       </c>
       <c r="J361">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="362" spans="1:10" x14ac:dyDescent="0.25">
@@ -11873,7 +11876,7 @@
         <v>79</v>
       </c>
       <c r="J362">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="363" spans="1:10" x14ac:dyDescent="0.25">
@@ -11902,7 +11905,7 @@
         <v>79</v>
       </c>
       <c r="J363">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="364" spans="1:10" x14ac:dyDescent="0.25">
@@ -11931,7 +11934,7 @@
         <v>79</v>
       </c>
       <c r="J364">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="365" spans="1:10" x14ac:dyDescent="0.25">
@@ -11960,7 +11963,7 @@
         <v>79</v>
       </c>
       <c r="J365">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="366" spans="1:10" x14ac:dyDescent="0.25">
@@ -11989,7 +11992,7 @@
         <v>79</v>
       </c>
       <c r="J366">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="367" spans="1:10" x14ac:dyDescent="0.25">
@@ -12018,7 +12021,7 @@
         <v>79</v>
       </c>
       <c r="J367">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="368" spans="1:10" x14ac:dyDescent="0.25">
@@ -12047,7 +12050,7 @@
         <v>79</v>
       </c>
       <c r="J368">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="369" spans="1:10" x14ac:dyDescent="0.25">
@@ -12076,7 +12079,7 @@
         <v>79</v>
       </c>
       <c r="J369">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="370" spans="1:10" x14ac:dyDescent="0.25">
@@ -12105,7 +12108,7 @@
         <v>79</v>
       </c>
       <c r="J370">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="371" spans="1:10" x14ac:dyDescent="0.25">
@@ -12134,7 +12137,7 @@
         <v>79</v>
       </c>
       <c r="J371">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="372" spans="1:10" x14ac:dyDescent="0.25">
@@ -12163,7 +12166,7 @@
         <v>79</v>
       </c>
       <c r="J372">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="373" spans="1:10" x14ac:dyDescent="0.25">
@@ -12192,7 +12195,7 @@
         <v>79</v>
       </c>
       <c r="J373">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="374" spans="1:10" x14ac:dyDescent="0.25">
@@ -12221,7 +12224,7 @@
         <v>79</v>
       </c>
       <c r="J374">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="375" spans="1:10" x14ac:dyDescent="0.25">
@@ -12250,7 +12253,7 @@
         <v>79</v>
       </c>
       <c r="J375">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="376" spans="1:10" x14ac:dyDescent="0.25">
@@ -12279,7 +12282,7 @@
         <v>79</v>
       </c>
       <c r="J376">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="377" spans="1:10" x14ac:dyDescent="0.25">
@@ -12308,7 +12311,7 @@
         <v>79</v>
       </c>
       <c r="J377">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="378" spans="1:10" x14ac:dyDescent="0.25">
@@ -12337,7 +12340,7 @@
         <v>79</v>
       </c>
       <c r="J378">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="379" spans="1:10" x14ac:dyDescent="0.25">
@@ -12366,7 +12369,7 @@
         <v>79</v>
       </c>
       <c r="J379">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="380" spans="1:10" x14ac:dyDescent="0.25">
@@ -12395,7 +12398,7 @@
         <v>79</v>
       </c>
       <c r="J380">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="381" spans="1:10" x14ac:dyDescent="0.25">
@@ -12424,6 +12427,876 @@
         <v>79</v>
       </c>
       <c r="J381">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>18</v>
+      </c>
+      <c r="B382">
+        <v>1</v>
+      </c>
+      <c r="C382" t="s">
+        <v>35</v>
+      </c>
+      <c r="D382">
+        <v>2.3488888888888888</v>
+      </c>
+      <c r="E382">
+        <v>10.31111111111111</v>
+      </c>
+      <c r="F382" t="s">
+        <v>0</v>
+      </c>
+      <c r="H382" t="s">
+        <v>115</v>
+      </c>
+      <c r="I382" t="s">
+        <v>79</v>
+      </c>
+      <c r="J382">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="383" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>18</v>
+      </c>
+      <c r="B383">
+        <v>2</v>
+      </c>
+      <c r="C383" t="s">
+        <v>35</v>
+      </c>
+      <c r="D383">
+        <v>-1.753125</v>
+      </c>
+      <c r="E383">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F383" t="s">
+        <v>1</v>
+      </c>
+      <c r="H383" t="s">
+        <v>115</v>
+      </c>
+      <c r="I383" t="s">
+        <v>79</v>
+      </c>
+      <c r="J383">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="384" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>44</v>
+      </c>
+      <c r="B384">
+        <v>1</v>
+      </c>
+      <c r="C384" t="s">
+        <v>36</v>
+      </c>
+      <c r="D384">
+        <v>-1.753125</v>
+      </c>
+      <c r="E384">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F384" t="s">
+        <v>1</v>
+      </c>
+      <c r="H384" t="s">
+        <v>115</v>
+      </c>
+      <c r="I384" t="s">
+        <v>79</v>
+      </c>
+      <c r="J384">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="385" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>44</v>
+      </c>
+      <c r="B385">
+        <v>2</v>
+      </c>
+      <c r="C385" t="s">
+        <v>36</v>
+      </c>
+      <c r="D385">
+        <v>-0.40769230769230752</v>
+      </c>
+      <c r="E385">
+        <v>21.388461538461538</v>
+      </c>
+      <c r="F385" t="s">
+        <v>2</v>
+      </c>
+      <c r="H385" t="s">
+        <v>115</v>
+      </c>
+      <c r="I385" t="s">
+        <v>79</v>
+      </c>
+      <c r="J385">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="386" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>21</v>
+      </c>
+      <c r="B386">
+        <v>1</v>
+      </c>
+      <c r="C386" t="s">
+        <v>35</v>
+      </c>
+      <c r="D386">
+        <v>-0.40769230769230752</v>
+      </c>
+      <c r="E386">
+        <v>21.388461538461538</v>
+      </c>
+      <c r="F386" t="s">
+        <v>2</v>
+      </c>
+      <c r="H386" t="s">
+        <v>115</v>
+      </c>
+      <c r="I386" t="s">
+        <v>79</v>
+      </c>
+      <c r="J386">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>21</v>
+      </c>
+      <c r="B387">
+        <v>2</v>
+      </c>
+      <c r="C387" t="s">
+        <v>35</v>
+      </c>
+      <c r="D387">
+        <v>-1.78</v>
+      </c>
+      <c r="E387">
+        <v>27.603999999999996</v>
+      </c>
+      <c r="F387" t="s">
+        <v>3</v>
+      </c>
+      <c r="H387" t="s">
+        <v>115</v>
+      </c>
+      <c r="I387" t="s">
+        <v>79</v>
+      </c>
+      <c r="J387">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="388" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>73</v>
+      </c>
+      <c r="B388">
+        <v>1</v>
+      </c>
+      <c r="C388" t="s">
+        <v>36</v>
+      </c>
+      <c r="D388">
+        <v>-1.78</v>
+      </c>
+      <c r="E388">
+        <v>27.603999999999996</v>
+      </c>
+      <c r="F388" t="s">
+        <v>3</v>
+      </c>
+      <c r="H388" t="s">
+        <v>115</v>
+      </c>
+      <c r="I388" t="s">
+        <v>79</v>
+      </c>
+      <c r="J388">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="389" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>73</v>
+      </c>
+      <c r="B389">
+        <v>2</v>
+      </c>
+      <c r="C389" t="s">
+        <v>36</v>
+      </c>
+      <c r="D389">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E389">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F389" t="s">
+        <v>9</v>
+      </c>
+      <c r="H389" t="s">
+        <v>115</v>
+      </c>
+      <c r="I389" t="s">
+        <v>79</v>
+      </c>
+      <c r="J389">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="390" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>28</v>
+      </c>
+      <c r="B390">
+        <v>1</v>
+      </c>
+      <c r="C390" t="s">
+        <v>35</v>
+      </c>
+      <c r="D390">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E390">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F390" t="s">
+        <v>9</v>
+      </c>
+      <c r="H390" t="s">
+        <v>115</v>
+      </c>
+      <c r="I390" t="s">
+        <v>79</v>
+      </c>
+      <c r="J390">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="391" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>28</v>
+      </c>
+      <c r="B391">
+        <v>2</v>
+      </c>
+      <c r="C391" t="s">
+        <v>35</v>
+      </c>
+      <c r="D391">
+        <v>-15.824999999999999</v>
+      </c>
+      <c r="E391">
+        <v>15.45</v>
+      </c>
+      <c r="F391" t="s">
+        <v>14</v>
+      </c>
+      <c r="H391" t="s">
+        <v>115</v>
+      </c>
+      <c r="I391" t="s">
+        <v>79</v>
+      </c>
+      <c r="J391">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="392" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>64</v>
+      </c>
+      <c r="B392">
+        <v>1</v>
+      </c>
+      <c r="C392" t="s">
+        <v>36</v>
+      </c>
+      <c r="D392">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E392">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F392" t="s">
+        <v>9</v>
+      </c>
+      <c r="H392" t="s">
+        <v>115</v>
+      </c>
+      <c r="I392" t="s">
+        <v>79</v>
+      </c>
+      <c r="J392">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="393" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>64</v>
+      </c>
+      <c r="B393">
+        <v>2</v>
+      </c>
+      <c r="C393" t="s">
+        <v>36</v>
+      </c>
+      <c r="D393">
+        <v>-9.16</v>
+      </c>
+      <c r="E393">
+        <v>26.439999999999998</v>
+      </c>
+      <c r="F393" t="s">
+        <v>10</v>
+      </c>
+      <c r="H393" t="s">
+        <v>115</v>
+      </c>
+      <c r="I393" t="s">
+        <v>79</v>
+      </c>
+      <c r="J393">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="394" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>29</v>
+      </c>
+      <c r="B394">
+        <v>1</v>
+      </c>
+      <c r="C394" t="s">
+        <v>36</v>
+      </c>
+      <c r="D394">
+        <v>-9.16</v>
+      </c>
+      <c r="E394">
+        <v>26.439999999999998</v>
+      </c>
+      <c r="F394" t="s">
+        <v>10</v>
+      </c>
+      <c r="H394" t="s">
+        <v>115</v>
+      </c>
+      <c r="I394" t="s">
+        <v>79</v>
+      </c>
+      <c r="J394">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="395" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>29</v>
+      </c>
+      <c r="B395">
+        <v>2</v>
+      </c>
+      <c r="C395" t="s">
+        <v>36</v>
+      </c>
+      <c r="D395">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E395">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F395" t="s">
+        <v>11</v>
+      </c>
+      <c r="H395" t="s">
+        <v>115</v>
+      </c>
+      <c r="I395" t="s">
+        <v>79</v>
+      </c>
+      <c r="J395">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="396" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>31</v>
+      </c>
+      <c r="B396">
+        <v>1</v>
+      </c>
+      <c r="C396" t="s">
+        <v>35</v>
+      </c>
+      <c r="D396">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E396">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F396" t="s">
+        <v>11</v>
+      </c>
+      <c r="H396" t="s">
+        <v>115</v>
+      </c>
+      <c r="I396" t="s">
+        <v>79</v>
+      </c>
+      <c r="J396">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="397" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>31</v>
+      </c>
+      <c r="B397">
+        <v>2</v>
+      </c>
+      <c r="C397" t="s">
+        <v>35</v>
+      </c>
+      <c r="D397">
+        <v>-13.557142857142859</v>
+      </c>
+      <c r="E397">
+        <v>33.514285714285712</v>
+      </c>
+      <c r="F397" t="s">
+        <v>12</v>
+      </c>
+      <c r="H397" t="s">
+        <v>115</v>
+      </c>
+      <c r="I397" t="s">
+        <v>79</v>
+      </c>
+      <c r="J397">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="398" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>32</v>
+      </c>
+      <c r="B398">
+        <v>1</v>
+      </c>
+      <c r="C398" t="s">
+        <v>35</v>
+      </c>
+      <c r="D398">
+        <v>-13.557142857142859</v>
+      </c>
+      <c r="E398">
+        <v>33.514285714285712</v>
+      </c>
+      <c r="F398" t="s">
+        <v>12</v>
+      </c>
+      <c r="H398" t="s">
+        <v>115</v>
+      </c>
+      <c r="I398" t="s">
+        <v>79</v>
+      </c>
+      <c r="J398">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="399" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A399" t="s">
+        <v>32</v>
+      </c>
+      <c r="B399">
+        <v>2</v>
+      </c>
+      <c r="C399" t="s">
+        <v>35</v>
+      </c>
+      <c r="D399">
+        <v>-13.3</v>
+      </c>
+      <c r="E399">
+        <v>39.125</v>
+      </c>
+      <c r="F399" t="s">
+        <v>13</v>
+      </c>
+      <c r="H399" t="s">
+        <v>115</v>
+      </c>
+      <c r="I399" t="s">
+        <v>79</v>
+      </c>
+      <c r="J399">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="400" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>30</v>
+      </c>
+      <c r="B400">
+        <v>1</v>
+      </c>
+      <c r="C400" t="s">
+        <v>36</v>
+      </c>
+      <c r="D400">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E400">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F400" t="s">
+        <v>11</v>
+      </c>
+      <c r="H400" t="s">
+        <v>115</v>
+      </c>
+      <c r="I400" t="s">
+        <v>79</v>
+      </c>
+      <c r="J400">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>30</v>
+      </c>
+      <c r="B401">
+        <v>2</v>
+      </c>
+      <c r="C401" t="s">
+        <v>36</v>
+      </c>
+      <c r="D401">
+        <v>-23.125</v>
+      </c>
+      <c r="E401">
+        <v>29.665624999999999</v>
+      </c>
+      <c r="F401" t="s">
+        <v>15</v>
+      </c>
+      <c r="H401" t="s">
+        <v>115</v>
+      </c>
+      <c r="I401" t="s">
+        <v>79</v>
+      </c>
+      <c r="J401">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="402" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>22</v>
+      </c>
+      <c r="B402">
+        <v>1</v>
+      </c>
+      <c r="C402" t="s">
+        <v>35</v>
+      </c>
+      <c r="D402">
+        <v>-1.78</v>
+      </c>
+      <c r="E402">
+        <v>27.603999999999996</v>
+      </c>
+      <c r="F402" t="s">
+        <v>3</v>
+      </c>
+      <c r="H402" t="s">
+        <v>115</v>
+      </c>
+      <c r="I402" t="s">
+        <v>79</v>
+      </c>
+      <c r="J402">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>22</v>
+      </c>
+      <c r="B403">
+        <v>2</v>
+      </c>
+      <c r="C403" t="s">
+        <v>35</v>
+      </c>
+      <c r="D403">
+        <v>-1.44444444444444</v>
+      </c>
+      <c r="E403">
+        <v>30.911111111111115</v>
+      </c>
+      <c r="F403" t="s">
+        <v>8</v>
+      </c>
+      <c r="H403" t="s">
+        <v>115</v>
+      </c>
+      <c r="I403" t="s">
+        <v>79</v>
+      </c>
+      <c r="J403">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="404" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>24</v>
+      </c>
+      <c r="B404">
+        <v>1</v>
+      </c>
+      <c r="C404" t="s">
+        <v>36</v>
+      </c>
+      <c r="D404">
+        <v>-1.44444444444444</v>
+      </c>
+      <c r="E404">
+        <v>30.911111111111115</v>
+      </c>
+      <c r="F404" t="s">
+        <v>8</v>
+      </c>
+      <c r="H404" t="s">
+        <v>115</v>
+      </c>
+      <c r="I404" t="s">
+        <v>79</v>
+      </c>
+      <c r="J404">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="405" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>24</v>
+      </c>
+      <c r="B405">
+        <v>2</v>
+      </c>
+      <c r="C405" t="s">
+        <v>36</v>
+      </c>
+      <c r="D405">
+        <v>-3.7333333333333329</v>
+      </c>
+      <c r="E405">
+        <v>33</v>
+      </c>
+      <c r="F405" t="s">
+        <v>5</v>
+      </c>
+      <c r="H405" t="s">
+        <v>115</v>
+      </c>
+      <c r="I405" t="s">
+        <v>79</v>
+      </c>
+      <c r="J405">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="406" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>25</v>
+      </c>
+      <c r="B406">
+        <v>1</v>
+      </c>
+      <c r="C406" t="s">
+        <v>36</v>
+      </c>
+      <c r="D406">
+        <v>-3.7333333333333329</v>
+      </c>
+      <c r="E406">
+        <v>33</v>
+      </c>
+      <c r="F406" t="s">
+        <v>5</v>
+      </c>
+      <c r="H406" t="s">
+        <v>115</v>
+      </c>
+      <c r="I406" t="s">
+        <v>79</v>
+      </c>
+      <c r="J406">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="407" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>25</v>
+      </c>
+      <c r="B407">
+        <v>2</v>
+      </c>
+      <c r="C407" t="s">
+        <v>36</v>
+      </c>
+      <c r="D407">
+        <v>-5.85</v>
+      </c>
+      <c r="E407">
+        <v>37.712499999999999</v>
+      </c>
+      <c r="F407" t="s">
+        <v>6</v>
+      </c>
+      <c r="H407" t="s">
+        <v>115</v>
+      </c>
+      <c r="I407" t="s">
+        <v>79</v>
+      </c>
+      <c r="J407">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="408" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A408" t="s">
+        <v>26</v>
+      </c>
+      <c r="B408">
+        <v>1</v>
+      </c>
+      <c r="C408" t="s">
+        <v>35</v>
+      </c>
+      <c r="D408">
+        <v>-5.85</v>
+      </c>
+      <c r="E408">
+        <v>37.712499999999999</v>
+      </c>
+      <c r="F408" t="s">
+        <v>6</v>
+      </c>
+      <c r="H408" t="s">
+        <v>115</v>
+      </c>
+      <c r="I408" t="s">
+        <v>79</v>
+      </c>
+      <c r="J408">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="409" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A409" t="s">
+        <v>26</v>
+      </c>
+      <c r="B409">
+        <v>2</v>
+      </c>
+      <c r="C409" t="s">
+        <v>35</v>
+      </c>
+      <c r="D409">
+        <v>-2.35</v>
+      </c>
+      <c r="E409">
+        <v>38.449999999999996</v>
+      </c>
+      <c r="F409" t="s">
+        <v>4</v>
+      </c>
+      <c r="H409" t="s">
+        <v>115</v>
+      </c>
+      <c r="I409" t="s">
+        <v>79</v>
+      </c>
+      <c r="J409">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="410" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A410" t="s">
+        <v>62</v>
+      </c>
+      <c r="B410">
+        <v>1</v>
+      </c>
+      <c r="C410" t="s">
+        <v>36</v>
+      </c>
+      <c r="D410">
+        <v>-0.40769230769230752</v>
+      </c>
+      <c r="E410">
+        <v>21.388461538461538</v>
+      </c>
+      <c r="F410" t="s">
+        <v>2</v>
+      </c>
+      <c r="H410" t="s">
+        <v>115</v>
+      </c>
+      <c r="I410" t="s">
+        <v>79</v>
+      </c>
+      <c r="J410">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="411" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A411" t="s">
+        <v>62</v>
+      </c>
+      <c r="B411">
+        <v>2</v>
+      </c>
+      <c r="C411" t="s">
+        <v>36</v>
+      </c>
+      <c r="D411">
+        <v>-5.5714285714285703</v>
+      </c>
+      <c r="E411">
+        <v>15.75</v>
+      </c>
+      <c r="F411" t="s">
+        <v>7</v>
+      </c>
+      <c r="H411" t="s">
+        <v>115</v>
+      </c>
+      <c r="I411" t="s">
+        <v>79</v>
+      </c>
+      <c r="J411">
         <v>1</v>
       </c>
     </row>
@@ -12438,7 +13311,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="A1:C18"/>
+      <selection activeCell="A2" sqref="A2:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add newest Ward bantu runs
</commit_message>
<xml_diff>
--- a/resources/datasets/MigratoryModel/CombinedMigratoryModel_GuthrieZone_Path - AllModels.xlsx
+++ b/resources/datasets/MigratoryModel/CombinedMigratoryModel_GuthrieZone_Path - AllModels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby Ford\Desktop\BantuMigration\Github\resources\datasets\MigratoryModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771C601A-7E53-4173-B214-E2DC6BB18105}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD127310-9C23-490F-9CFB-F021EEAB34F8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{48220AAF-5FA7-46D3-8056-2130CE6EF7AB}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2000" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2150" uniqueCount="120">
   <si>
     <t>A</t>
   </si>
@@ -377,6 +377,18 @@
   </si>
   <si>
     <t>AMNH - Combined 400 (all 5) - H</t>
+  </si>
+  <si>
+    <t>D-E</t>
+  </si>
+  <si>
+    <t>E-J</t>
+  </si>
+  <si>
+    <t>E-L</t>
+  </si>
+  <si>
+    <t>AMNH - Combined 400 -11-H</t>
   </si>
 </sst>
 </file>
@@ -728,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB7D369B-DF5B-472F-B73D-7CCA41A92755}">
-  <dimension ref="A1:J411"/>
+  <dimension ref="A1:J441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A350" workbookViewId="0">
-      <selection activeCell="L383" sqref="L383"/>
+    <sheetView tabSelected="1" topLeftCell="A405" workbookViewId="0">
+      <selection activeCell="H428" sqref="H428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13300,6 +13312,876 @@
         <v>1</v>
       </c>
     </row>
+    <row r="412" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A412" t="s">
+        <v>18</v>
+      </c>
+      <c r="B412">
+        <v>1</v>
+      </c>
+      <c r="C412" t="s">
+        <v>35</v>
+      </c>
+      <c r="D412">
+        <v>2.3488888888888888</v>
+      </c>
+      <c r="E412">
+        <v>10.31111111111111</v>
+      </c>
+      <c r="F412" t="s">
+        <v>0</v>
+      </c>
+      <c r="H412" t="s">
+        <v>119</v>
+      </c>
+      <c r="I412" t="s">
+        <v>79</v>
+      </c>
+      <c r="J412">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="413" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A413" t="s">
+        <v>18</v>
+      </c>
+      <c r="B413">
+        <v>2</v>
+      </c>
+      <c r="C413" t="s">
+        <v>35</v>
+      </c>
+      <c r="D413">
+        <v>-1.753125</v>
+      </c>
+      <c r="E413">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F413" t="s">
+        <v>1</v>
+      </c>
+      <c r="H413" t="s">
+        <v>119</v>
+      </c>
+      <c r="I413" t="s">
+        <v>79</v>
+      </c>
+      <c r="J413">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="414" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A414" t="s">
+        <v>19</v>
+      </c>
+      <c r="B414">
+        <v>1</v>
+      </c>
+      <c r="C414" t="s">
+        <v>35</v>
+      </c>
+      <c r="D414">
+        <v>-1.753125</v>
+      </c>
+      <c r="E414">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F414" t="s">
+        <v>1</v>
+      </c>
+      <c r="H414" t="s">
+        <v>119</v>
+      </c>
+      <c r="I414" t="s">
+        <v>79</v>
+      </c>
+      <c r="J414">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="415" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A415" t="s">
+        <v>19</v>
+      </c>
+      <c r="B415">
+        <v>2</v>
+      </c>
+      <c r="C415" t="s">
+        <v>35</v>
+      </c>
+      <c r="D415">
+        <v>-5.5714285714285703</v>
+      </c>
+      <c r="E415">
+        <v>15.75</v>
+      </c>
+      <c r="F415" t="s">
+        <v>7</v>
+      </c>
+      <c r="H415" t="s">
+        <v>119</v>
+      </c>
+      <c r="I415" t="s">
+        <v>79</v>
+      </c>
+      <c r="J415">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="416" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>44</v>
+      </c>
+      <c r="B416">
+        <v>1</v>
+      </c>
+      <c r="C416" t="s">
+        <v>35</v>
+      </c>
+      <c r="D416">
+        <v>-1.753125</v>
+      </c>
+      <c r="E416">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F416" t="s">
+        <v>1</v>
+      </c>
+      <c r="H416" t="s">
+        <v>119</v>
+      </c>
+      <c r="I416" t="s">
+        <v>79</v>
+      </c>
+      <c r="J416">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="417" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A417" t="s">
+        <v>44</v>
+      </c>
+      <c r="B417">
+        <v>2</v>
+      </c>
+      <c r="C417" t="s">
+        <v>35</v>
+      </c>
+      <c r="D417">
+        <v>-0.40769230769230752</v>
+      </c>
+      <c r="E417">
+        <v>21.388461538461538</v>
+      </c>
+      <c r="F417" t="s">
+        <v>2</v>
+      </c>
+      <c r="H417" t="s">
+        <v>119</v>
+      </c>
+      <c r="I417" t="s">
+        <v>79</v>
+      </c>
+      <c r="J417">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="418" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
+        <v>21</v>
+      </c>
+      <c r="B418">
+        <v>1</v>
+      </c>
+      <c r="C418" t="s">
+        <v>36</v>
+      </c>
+      <c r="D418">
+        <v>-0.40769230769230752</v>
+      </c>
+      <c r="E418">
+        <v>21.388461538461538</v>
+      </c>
+      <c r="F418" t="s">
+        <v>2</v>
+      </c>
+      <c r="H418" t="s">
+        <v>119</v>
+      </c>
+      <c r="I418" t="s">
+        <v>79</v>
+      </c>
+      <c r="J418">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="419" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>21</v>
+      </c>
+      <c r="B419">
+        <v>2</v>
+      </c>
+      <c r="C419" t="s">
+        <v>36</v>
+      </c>
+      <c r="D419">
+        <v>-1.78</v>
+      </c>
+      <c r="E419">
+        <v>27.603999999999996</v>
+      </c>
+      <c r="F419" t="s">
+        <v>3</v>
+      </c>
+      <c r="H419" t="s">
+        <v>119</v>
+      </c>
+      <c r="I419" t="s">
+        <v>79</v>
+      </c>
+      <c r="J419">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="420" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A420" t="s">
+        <v>116</v>
+      </c>
+      <c r="B420">
+        <v>1</v>
+      </c>
+      <c r="C420" t="s">
+        <v>36</v>
+      </c>
+      <c r="D420">
+        <v>-1.78</v>
+      </c>
+      <c r="E420">
+        <v>27.603999999999996</v>
+      </c>
+      <c r="F420" t="s">
+        <v>3</v>
+      </c>
+      <c r="H420" t="s">
+        <v>119</v>
+      </c>
+      <c r="I420" t="s">
+        <v>79</v>
+      </c>
+      <c r="J420">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="421" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A421" t="s">
+        <v>116</v>
+      </c>
+      <c r="B421">
+        <v>2</v>
+      </c>
+      <c r="C421" t="s">
+        <v>36</v>
+      </c>
+      <c r="D421">
+        <v>-2.35</v>
+      </c>
+      <c r="E421">
+        <v>38.449999999999996</v>
+      </c>
+      <c r="F421" t="s">
+        <v>4</v>
+      </c>
+      <c r="H421" t="s">
+        <v>119</v>
+      </c>
+      <c r="I421" t="s">
+        <v>79</v>
+      </c>
+      <c r="J421">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="422" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>71</v>
+      </c>
+      <c r="B422">
+        <v>1</v>
+      </c>
+      <c r="C422" t="s">
+        <v>36</v>
+      </c>
+      <c r="D422">
+        <v>-1.78</v>
+      </c>
+      <c r="E422">
+        <v>27.603999999999996</v>
+      </c>
+      <c r="F422" t="s">
+        <v>3</v>
+      </c>
+      <c r="H422" t="s">
+        <v>119</v>
+      </c>
+      <c r="I422" t="s">
+        <v>79</v>
+      </c>
+      <c r="J422">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="423" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A423" t="s">
+        <v>71</v>
+      </c>
+      <c r="B423">
+        <v>2</v>
+      </c>
+      <c r="C423" t="s">
+        <v>36</v>
+      </c>
+      <c r="D423">
+        <v>-5.85</v>
+      </c>
+      <c r="E423">
+        <v>37.712499999999999</v>
+      </c>
+      <c r="F423" t="s">
+        <v>6</v>
+      </c>
+      <c r="H423" t="s">
+        <v>119</v>
+      </c>
+      <c r="I423" t="s">
+        <v>79</v>
+      </c>
+      <c r="J423">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="424" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>72</v>
+      </c>
+      <c r="B424">
+        <v>1</v>
+      </c>
+      <c r="C424" t="s">
+        <v>36</v>
+      </c>
+      <c r="D424">
+        <v>-2.35</v>
+      </c>
+      <c r="E424">
+        <v>38.449999999999996</v>
+      </c>
+      <c r="F424" t="s">
+        <v>4</v>
+      </c>
+      <c r="H424" t="s">
+        <v>119</v>
+      </c>
+      <c r="I424" t="s">
+        <v>79</v>
+      </c>
+      <c r="J424">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="425" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>72</v>
+      </c>
+      <c r="B425">
+        <v>2</v>
+      </c>
+      <c r="C425" t="s">
+        <v>36</v>
+      </c>
+      <c r="D425">
+        <v>-3.7333333333333329</v>
+      </c>
+      <c r="E425">
+        <v>33</v>
+      </c>
+      <c r="F425" t="s">
+        <v>5</v>
+      </c>
+      <c r="H425" t="s">
+        <v>119</v>
+      </c>
+      <c r="I425" t="s">
+        <v>79</v>
+      </c>
+      <c r="J425">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="426" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>117</v>
+      </c>
+      <c r="B426">
+        <v>1</v>
+      </c>
+      <c r="C426" t="s">
+        <v>36</v>
+      </c>
+      <c r="D426">
+        <v>-2.35</v>
+      </c>
+      <c r="E426">
+        <v>38.449999999999996</v>
+      </c>
+      <c r="F426" t="s">
+        <v>4</v>
+      </c>
+      <c r="H426" t="s">
+        <v>119</v>
+      </c>
+      <c r="I426" t="s">
+        <v>79</v>
+      </c>
+      <c r="J426">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="427" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>117</v>
+      </c>
+      <c r="B427">
+        <v>2</v>
+      </c>
+      <c r="C427" t="s">
+        <v>36</v>
+      </c>
+      <c r="D427">
+        <v>-1.44444444444444</v>
+      </c>
+      <c r="E427">
+        <v>30.911111111111115</v>
+      </c>
+      <c r="F427" t="s">
+        <v>8</v>
+      </c>
+      <c r="H427" t="s">
+        <v>119</v>
+      </c>
+      <c r="I427" t="s">
+        <v>79</v>
+      </c>
+      <c r="J427">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="428" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>118</v>
+      </c>
+      <c r="B428">
+        <v>1</v>
+      </c>
+      <c r="C428" t="s">
+        <v>36</v>
+      </c>
+      <c r="D428">
+        <v>-2.35</v>
+      </c>
+      <c r="E428">
+        <v>38.449999999999996</v>
+      </c>
+      <c r="F428" t="s">
+        <v>4</v>
+      </c>
+      <c r="H428" t="s">
+        <v>119</v>
+      </c>
+      <c r="I428" t="s">
+        <v>79</v>
+      </c>
+      <c r="J428">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="429" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A429" t="s">
+        <v>118</v>
+      </c>
+      <c r="B429">
+        <v>2</v>
+      </c>
+      <c r="C429" t="s">
+        <v>36</v>
+      </c>
+      <c r="D429">
+        <v>-9.16</v>
+      </c>
+      <c r="E429">
+        <v>26.439999999999998</v>
+      </c>
+      <c r="F429" t="s">
+        <v>10</v>
+      </c>
+      <c r="H429" t="s">
+        <v>119</v>
+      </c>
+      <c r="I429" t="s">
+        <v>79</v>
+      </c>
+      <c r="J429">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="430" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>27</v>
+      </c>
+      <c r="B430">
+        <v>1</v>
+      </c>
+      <c r="C430" t="s">
+        <v>35</v>
+      </c>
+      <c r="D430">
+        <v>-9.16</v>
+      </c>
+      <c r="E430">
+        <v>26.439999999999998</v>
+      </c>
+      <c r="F430" t="s">
+        <v>10</v>
+      </c>
+      <c r="H430" t="s">
+        <v>119</v>
+      </c>
+      <c r="I430" t="s">
+        <v>79</v>
+      </c>
+      <c r="J430">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="431" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>27</v>
+      </c>
+      <c r="B431">
+        <v>2</v>
+      </c>
+      <c r="C431" t="s">
+        <v>35</v>
+      </c>
+      <c r="D431">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E431">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F431" t="s">
+        <v>9</v>
+      </c>
+      <c r="H431" t="s">
+        <v>119</v>
+      </c>
+      <c r="I431" t="s">
+        <v>79</v>
+      </c>
+      <c r="J431">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="432" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>28</v>
+      </c>
+      <c r="B432">
+        <v>1</v>
+      </c>
+      <c r="C432" t="s">
+        <v>35</v>
+      </c>
+      <c r="D432">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E432">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F432" t="s">
+        <v>9</v>
+      </c>
+      <c r="H432" t="s">
+        <v>119</v>
+      </c>
+      <c r="I432" t="s">
+        <v>79</v>
+      </c>
+      <c r="J432">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="433" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>28</v>
+      </c>
+      <c r="B433">
+        <v>2</v>
+      </c>
+      <c r="C433" t="s">
+        <v>35</v>
+      </c>
+      <c r="D433">
+        <v>-15.824999999999999</v>
+      </c>
+      <c r="E433">
+        <v>15.45</v>
+      </c>
+      <c r="F433" t="s">
+        <v>14</v>
+      </c>
+      <c r="H433" t="s">
+        <v>119</v>
+      </c>
+      <c r="I433" t="s">
+        <v>79</v>
+      </c>
+      <c r="J433">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="434" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>29</v>
+      </c>
+      <c r="B434">
+        <v>1</v>
+      </c>
+      <c r="C434" t="s">
+        <v>35</v>
+      </c>
+      <c r="D434">
+        <v>-9.16</v>
+      </c>
+      <c r="E434">
+        <v>26.439999999999998</v>
+      </c>
+      <c r="F434" t="s">
+        <v>10</v>
+      </c>
+      <c r="H434" t="s">
+        <v>119</v>
+      </c>
+      <c r="I434" t="s">
+        <v>79</v>
+      </c>
+      <c r="J434">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="435" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>29</v>
+      </c>
+      <c r="B435">
+        <v>2</v>
+      </c>
+      <c r="C435" t="s">
+        <v>35</v>
+      </c>
+      <c r="D435">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E435">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F435" t="s">
+        <v>11</v>
+      </c>
+      <c r="H435" t="s">
+        <v>119</v>
+      </c>
+      <c r="I435" t="s">
+        <v>79</v>
+      </c>
+      <c r="J435">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="436" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>31</v>
+      </c>
+      <c r="B436">
+        <v>1</v>
+      </c>
+      <c r="C436" t="s">
+        <v>35</v>
+      </c>
+      <c r="D436">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E436">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F436" t="s">
+        <v>11</v>
+      </c>
+      <c r="H436" t="s">
+        <v>119</v>
+      </c>
+      <c r="I436" t="s">
+        <v>79</v>
+      </c>
+      <c r="J436">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="437" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>31</v>
+      </c>
+      <c r="B437">
+        <v>2</v>
+      </c>
+      <c r="C437" t="s">
+        <v>35</v>
+      </c>
+      <c r="D437">
+        <v>-13.557142857142859</v>
+      </c>
+      <c r="E437">
+        <v>33.514285714285712</v>
+      </c>
+      <c r="F437" t="s">
+        <v>12</v>
+      </c>
+      <c r="H437" t="s">
+        <v>119</v>
+      </c>
+      <c r="I437" t="s">
+        <v>79</v>
+      </c>
+      <c r="J437">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="438" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
+        <v>32</v>
+      </c>
+      <c r="B438">
+        <v>1</v>
+      </c>
+      <c r="C438" t="s">
+        <v>35</v>
+      </c>
+      <c r="D438">
+        <v>-13.557142857142859</v>
+      </c>
+      <c r="E438">
+        <v>33.514285714285712</v>
+      </c>
+      <c r="F438" t="s">
+        <v>12</v>
+      </c>
+      <c r="H438" t="s">
+        <v>119</v>
+      </c>
+      <c r="I438" t="s">
+        <v>79</v>
+      </c>
+      <c r="J438">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="439" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>32</v>
+      </c>
+      <c r="B439">
+        <v>2</v>
+      </c>
+      <c r="C439" t="s">
+        <v>35</v>
+      </c>
+      <c r="D439">
+        <v>-13.3</v>
+      </c>
+      <c r="E439">
+        <v>39.125</v>
+      </c>
+      <c r="F439" t="s">
+        <v>13</v>
+      </c>
+      <c r="H439" t="s">
+        <v>119</v>
+      </c>
+      <c r="I439" t="s">
+        <v>79</v>
+      </c>
+      <c r="J439">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="440" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>30</v>
+      </c>
+      <c r="B440">
+        <v>1</v>
+      </c>
+      <c r="C440" t="s">
+        <v>35</v>
+      </c>
+      <c r="D440">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E440">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F440" t="s">
+        <v>11</v>
+      </c>
+      <c r="H440" t="s">
+        <v>119</v>
+      </c>
+      <c r="I440" t="s">
+        <v>79</v>
+      </c>
+      <c r="J440">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="441" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>30</v>
+      </c>
+      <c r="B441">
+        <v>2</v>
+      </c>
+      <c r="C441" t="s">
+        <v>35</v>
+      </c>
+      <c r="D441">
+        <v>-23.125</v>
+      </c>
+      <c r="E441">
+        <v>29.665624999999999</v>
+      </c>
+      <c r="F441" t="s">
+        <v>15</v>
+      </c>
+      <c r="H441" t="s">
+        <v>119</v>
+      </c>
+      <c r="I441" t="s">
+        <v>79</v>
+      </c>
+      <c r="J441">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J381" xr:uid="{303E4824-0DA0-4156-A165-CC92066081A2}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add Ward's new models (`lang-sw-11-H` and `lang-sw-all5-H`)
</commit_message>
<xml_diff>
--- a/resources/datasets/MigratoryModel/CombinedMigratoryModel_GuthrieZone_Path - AllModels.xlsx
+++ b/resources/datasets/MigratoryModel/CombinedMigratoryModel_GuthrieZone_Path - AllModels.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby Ford\Desktop\BantuMigration\Github\resources\datasets\MigratoryModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD127310-9C23-490F-9CFB-F021EEAB34F8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD91C202-3064-4B34-A289-8C5267BE303E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{48220AAF-5FA7-46D3-8056-2130CE6EF7AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48220AAF-5FA7-46D3-8056-2130CE6EF7AB}"/>
   </bookViews>
   <sheets>
     <sheet name="MigratoryModel_TableauData" sheetId="1" r:id="rId1"/>
     <sheet name="ZoneCenterLocations" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MigratoryModel_TableauData!$A$1:$J$381</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MigratoryModel_TableauData!$A$1:$J$501</definedName>
   </definedNames>
   <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2150" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2450" uniqueCount="123">
   <si>
     <t>A</t>
   </si>
@@ -390,6 +390,15 @@
   <si>
     <t>AMNH - Combined 400 -11-H</t>
   </si>
+  <si>
+    <t>new-jan_lang-sw-11-H</t>
+  </si>
+  <si>
+    <t>N-M</t>
+  </si>
+  <si>
+    <t>new-jan_lang-sw-all5-H</t>
+  </si>
 </sst>
 </file>
 
@@ -740,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB7D369B-DF5B-472F-B73D-7CCA41A92755}">
-  <dimension ref="A1:J441"/>
+  <dimension ref="A1:J501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A405" workbookViewId="0">
-      <selection activeCell="H428" sqref="H428"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F455" sqref="F455"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14182,8 +14191,1748 @@
         <v>1</v>
       </c>
     </row>
+    <row r="442" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>18</v>
+      </c>
+      <c r="B442">
+        <v>1</v>
+      </c>
+      <c r="C442" t="s">
+        <v>35</v>
+      </c>
+      <c r="D442">
+        <v>2.3488888888888888</v>
+      </c>
+      <c r="E442">
+        <v>10.31111111111111</v>
+      </c>
+      <c r="F442" t="s">
+        <v>0</v>
+      </c>
+      <c r="H442" t="s">
+        <v>120</v>
+      </c>
+      <c r="I442" t="s">
+        <v>79</v>
+      </c>
+      <c r="J442">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="443" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>18</v>
+      </c>
+      <c r="B443">
+        <v>2</v>
+      </c>
+      <c r="C443" t="s">
+        <v>35</v>
+      </c>
+      <c r="D443">
+        <v>-1.753125</v>
+      </c>
+      <c r="E443">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F443" t="s">
+        <v>1</v>
+      </c>
+      <c r="H443" t="s">
+        <v>120</v>
+      </c>
+      <c r="I443" t="s">
+        <v>79</v>
+      </c>
+      <c r="J443">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="444" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>19</v>
+      </c>
+      <c r="B444">
+        <v>1</v>
+      </c>
+      <c r="C444" t="s">
+        <v>35</v>
+      </c>
+      <c r="D444">
+        <v>-1.753125</v>
+      </c>
+      <c r="E444">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F444" t="s">
+        <v>1</v>
+      </c>
+      <c r="H444" t="s">
+        <v>120</v>
+      </c>
+      <c r="I444" t="s">
+        <v>79</v>
+      </c>
+      <c r="J444">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="445" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>19</v>
+      </c>
+      <c r="B445">
+        <v>2</v>
+      </c>
+      <c r="C445" t="s">
+        <v>35</v>
+      </c>
+      <c r="D445">
+        <v>-5.5714285714285703</v>
+      </c>
+      <c r="E445">
+        <v>15.75</v>
+      </c>
+      <c r="F445" t="s">
+        <v>7</v>
+      </c>
+      <c r="H445" t="s">
+        <v>120</v>
+      </c>
+      <c r="I445" t="s">
+        <v>79</v>
+      </c>
+      <c r="J445">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="446" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>44</v>
+      </c>
+      <c r="B446">
+        <v>1</v>
+      </c>
+      <c r="C446" t="s">
+        <v>35</v>
+      </c>
+      <c r="D446">
+        <v>-1.753125</v>
+      </c>
+      <c r="E446">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F446" t="s">
+        <v>1</v>
+      </c>
+      <c r="H446" t="s">
+        <v>120</v>
+      </c>
+      <c r="I446" t="s">
+        <v>79</v>
+      </c>
+      <c r="J446">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="447" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>44</v>
+      </c>
+      <c r="B447">
+        <v>2</v>
+      </c>
+      <c r="C447" t="s">
+        <v>35</v>
+      </c>
+      <c r="D447">
+        <v>-0.40769230769230752</v>
+      </c>
+      <c r="E447">
+        <v>21.388461538461538</v>
+      </c>
+      <c r="F447" t="s">
+        <v>2</v>
+      </c>
+      <c r="H447" t="s">
+        <v>120</v>
+      </c>
+      <c r="I447" t="s">
+        <v>79</v>
+      </c>
+      <c r="J447">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="448" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A448" t="s">
+        <v>21</v>
+      </c>
+      <c r="B448">
+        <v>1</v>
+      </c>
+      <c r="C448" t="s">
+        <v>36</v>
+      </c>
+      <c r="D448">
+        <v>-0.40769230769230752</v>
+      </c>
+      <c r="E448">
+        <v>21.388461538461538</v>
+      </c>
+      <c r="F448" t="s">
+        <v>2</v>
+      </c>
+      <c r="H448" t="s">
+        <v>120</v>
+      </c>
+      <c r="I448" t="s">
+        <v>79</v>
+      </c>
+      <c r="J448">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="449" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>21</v>
+      </c>
+      <c r="B449">
+        <v>2</v>
+      </c>
+      <c r="C449" t="s">
+        <v>36</v>
+      </c>
+      <c r="D449">
+        <v>-1.78</v>
+      </c>
+      <c r="E449">
+        <v>27.603999999999996</v>
+      </c>
+      <c r="F449" t="s">
+        <v>3</v>
+      </c>
+      <c r="H449" t="s">
+        <v>120</v>
+      </c>
+      <c r="I449" t="s">
+        <v>79</v>
+      </c>
+      <c r="J449">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="450" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A450" t="s">
+        <v>22</v>
+      </c>
+      <c r="B450">
+        <v>1</v>
+      </c>
+      <c r="C450" t="s">
+        <v>36</v>
+      </c>
+      <c r="D450">
+        <v>-1.78</v>
+      </c>
+      <c r="E450">
+        <v>27.603999999999996</v>
+      </c>
+      <c r="F450" t="s">
+        <v>3</v>
+      </c>
+      <c r="H450" t="s">
+        <v>120</v>
+      </c>
+      <c r="I450" t="s">
+        <v>79</v>
+      </c>
+      <c r="J450">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="451" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>22</v>
+      </c>
+      <c r="B451">
+        <v>2</v>
+      </c>
+      <c r="C451" t="s">
+        <v>36</v>
+      </c>
+      <c r="D451">
+        <v>-1.44444444444444</v>
+      </c>
+      <c r="E451">
+        <v>30.911111111111115</v>
+      </c>
+      <c r="F451" t="s">
+        <v>8</v>
+      </c>
+      <c r="H451" t="s">
+        <v>120</v>
+      </c>
+      <c r="I451" t="s">
+        <v>79</v>
+      </c>
+      <c r="J451">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="452" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>24</v>
+      </c>
+      <c r="B452">
+        <v>1</v>
+      </c>
+      <c r="C452" t="s">
+        <v>35</v>
+      </c>
+      <c r="D452">
+        <v>-1.44444444444444</v>
+      </c>
+      <c r="E452">
+        <v>30.911111111111115</v>
+      </c>
+      <c r="F452" t="s">
+        <v>8</v>
+      </c>
+      <c r="H452" t="s">
+        <v>120</v>
+      </c>
+      <c r="I452" t="s">
+        <v>79</v>
+      </c>
+      <c r="J452">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="453" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
+        <v>24</v>
+      </c>
+      <c r="B453">
+        <v>2</v>
+      </c>
+      <c r="C453" t="s">
+        <v>35</v>
+      </c>
+      <c r="D453">
+        <v>-3.7333333333333329</v>
+      </c>
+      <c r="E453">
+        <v>33</v>
+      </c>
+      <c r="F453" t="s">
+        <v>5</v>
+      </c>
+      <c r="H453" t="s">
+        <v>120</v>
+      </c>
+      <c r="I453" t="s">
+        <v>79</v>
+      </c>
+      <c r="J453">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="454" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
+        <v>25</v>
+      </c>
+      <c r="B454">
+        <v>1</v>
+      </c>
+      <c r="C454" t="s">
+        <v>36</v>
+      </c>
+      <c r="D454">
+        <v>-3.7333333333333329</v>
+      </c>
+      <c r="E454">
+        <v>33</v>
+      </c>
+      <c r="F454" t="s">
+        <v>5</v>
+      </c>
+      <c r="H454" t="s">
+        <v>120</v>
+      </c>
+      <c r="I454" t="s">
+        <v>79</v>
+      </c>
+      <c r="J454">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="455" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>25</v>
+      </c>
+      <c r="B455">
+        <v>2</v>
+      </c>
+      <c r="C455" t="s">
+        <v>36</v>
+      </c>
+      <c r="D455">
+        <v>-5.85</v>
+      </c>
+      <c r="E455">
+        <v>37.712499999999999</v>
+      </c>
+      <c r="F455" t="s">
+        <v>6</v>
+      </c>
+      <c r="H455" t="s">
+        <v>120</v>
+      </c>
+      <c r="I455" t="s">
+        <v>79</v>
+      </c>
+      <c r="J455">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="456" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>26</v>
+      </c>
+      <c r="B456">
+        <v>1</v>
+      </c>
+      <c r="C456" t="s">
+        <v>35</v>
+      </c>
+      <c r="D456">
+        <v>-5.85</v>
+      </c>
+      <c r="E456">
+        <v>37.712499999999999</v>
+      </c>
+      <c r="F456" t="s">
+        <v>6</v>
+      </c>
+      <c r="H456" t="s">
+        <v>120</v>
+      </c>
+      <c r="I456" t="s">
+        <v>79</v>
+      </c>
+      <c r="J456">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="457" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>26</v>
+      </c>
+      <c r="B457">
+        <v>2</v>
+      </c>
+      <c r="C457" t="s">
+        <v>35</v>
+      </c>
+      <c r="D457">
+        <v>-2.35</v>
+      </c>
+      <c r="E457">
+        <v>38.449999999999996</v>
+      </c>
+      <c r="F457" t="s">
+        <v>4</v>
+      </c>
+      <c r="H457" t="s">
+        <v>120</v>
+      </c>
+      <c r="I457" t="s">
+        <v>79</v>
+      </c>
+      <c r="J457">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="458" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>66</v>
+      </c>
+      <c r="B458">
+        <v>1</v>
+      </c>
+      <c r="C458" t="s">
+        <v>36</v>
+      </c>
+      <c r="D458">
+        <v>-5.85</v>
+      </c>
+      <c r="E458">
+        <v>37.712499999999999</v>
+      </c>
+      <c r="F458" t="s">
+        <v>6</v>
+      </c>
+      <c r="H458" t="s">
+        <v>120</v>
+      </c>
+      <c r="I458" t="s">
+        <v>79</v>
+      </c>
+      <c r="J458">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="459" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>66</v>
+      </c>
+      <c r="B459">
+        <v>2</v>
+      </c>
+      <c r="C459" t="s">
+        <v>36</v>
+      </c>
+      <c r="D459">
+        <v>-13.557142857142859</v>
+      </c>
+      <c r="E459">
+        <v>33.514285714285712</v>
+      </c>
+      <c r="F459" t="s">
+        <v>12</v>
+      </c>
+      <c r="H459" t="s">
+        <v>120</v>
+      </c>
+      <c r="I459" t="s">
+        <v>79</v>
+      </c>
+      <c r="J459">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="460" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>121</v>
+      </c>
+      <c r="B460">
+        <v>1</v>
+      </c>
+      <c r="C460" t="s">
+        <v>35</v>
+      </c>
+      <c r="D460">
+        <v>-13.557142857142859</v>
+      </c>
+      <c r="E460">
+        <v>33.514285714285712</v>
+      </c>
+      <c r="F460" t="s">
+        <v>12</v>
+      </c>
+      <c r="H460" t="s">
+        <v>120</v>
+      </c>
+      <c r="I460" t="s">
+        <v>79</v>
+      </c>
+      <c r="J460">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="461" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>121</v>
+      </c>
+      <c r="B461">
+        <v>2</v>
+      </c>
+      <c r="C461" t="s">
+        <v>35</v>
+      </c>
+      <c r="D461">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E461">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F461" t="s">
+        <v>11</v>
+      </c>
+      <c r="H461" t="s">
+        <v>120</v>
+      </c>
+      <c r="I461" t="s">
+        <v>79</v>
+      </c>
+      <c r="J461">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="462" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>53</v>
+      </c>
+      <c r="B462">
+        <v>1</v>
+      </c>
+      <c r="C462" t="s">
+        <v>35</v>
+      </c>
+      <c r="D462">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E462">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F462" t="s">
+        <v>11</v>
+      </c>
+      <c r="H462" t="s">
+        <v>120</v>
+      </c>
+      <c r="I462" t="s">
+        <v>79</v>
+      </c>
+      <c r="J462">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="463" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>53</v>
+      </c>
+      <c r="B463">
+        <v>2</v>
+      </c>
+      <c r="C463" t="s">
+        <v>35</v>
+      </c>
+      <c r="D463">
+        <v>-9.16</v>
+      </c>
+      <c r="E463">
+        <v>26.439999999999998</v>
+      </c>
+      <c r="F463" t="s">
+        <v>10</v>
+      </c>
+      <c r="H463" t="s">
+        <v>120</v>
+      </c>
+      <c r="I463" t="s">
+        <v>79</v>
+      </c>
+      <c r="J463">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="464" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>27</v>
+      </c>
+      <c r="B464">
+        <v>1</v>
+      </c>
+      <c r="C464" t="s">
+        <v>35</v>
+      </c>
+      <c r="D464">
+        <v>-9.16</v>
+      </c>
+      <c r="E464">
+        <v>26.439999999999998</v>
+      </c>
+      <c r="F464" t="s">
+        <v>10</v>
+      </c>
+      <c r="H464" t="s">
+        <v>120</v>
+      </c>
+      <c r="I464" t="s">
+        <v>79</v>
+      </c>
+      <c r="J464">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="465" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>27</v>
+      </c>
+      <c r="B465">
+        <v>2</v>
+      </c>
+      <c r="C465" t="s">
+        <v>35</v>
+      </c>
+      <c r="D465">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E465">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F465" t="s">
+        <v>9</v>
+      </c>
+      <c r="H465" t="s">
+        <v>120</v>
+      </c>
+      <c r="I465" t="s">
+        <v>79</v>
+      </c>
+      <c r="J465">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="466" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>28</v>
+      </c>
+      <c r="B466">
+        <v>1</v>
+      </c>
+      <c r="C466" t="s">
+        <v>35</v>
+      </c>
+      <c r="D466">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E466">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F466" t="s">
+        <v>9</v>
+      </c>
+      <c r="H466" t="s">
+        <v>120</v>
+      </c>
+      <c r="I466" t="s">
+        <v>79</v>
+      </c>
+      <c r="J466">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="467" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>28</v>
+      </c>
+      <c r="B467">
+        <v>2</v>
+      </c>
+      <c r="C467" t="s">
+        <v>35</v>
+      </c>
+      <c r="D467">
+        <v>-15.824999999999999</v>
+      </c>
+      <c r="E467">
+        <v>15.45</v>
+      </c>
+      <c r="F467" t="s">
+        <v>14</v>
+      </c>
+      <c r="H467" t="s">
+        <v>120</v>
+      </c>
+      <c r="I467" t="s">
+        <v>79</v>
+      </c>
+      <c r="J467">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="468" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>30</v>
+      </c>
+      <c r="B468">
+        <v>1</v>
+      </c>
+      <c r="C468" t="s">
+        <v>35</v>
+      </c>
+      <c r="D468">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E468">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F468" t="s">
+        <v>11</v>
+      </c>
+      <c r="H468" t="s">
+        <v>120</v>
+      </c>
+      <c r="I468" t="s">
+        <v>79</v>
+      </c>
+      <c r="J468">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="469" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>30</v>
+      </c>
+      <c r="B469">
+        <v>2</v>
+      </c>
+      <c r="C469" t="s">
+        <v>35</v>
+      </c>
+      <c r="D469">
+        <v>-23.125</v>
+      </c>
+      <c r="E469">
+        <v>29.665624999999999</v>
+      </c>
+      <c r="F469" t="s">
+        <v>15</v>
+      </c>
+      <c r="H469" t="s">
+        <v>120</v>
+      </c>
+      <c r="I469" t="s">
+        <v>79</v>
+      </c>
+      <c r="J469">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="470" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>32</v>
+      </c>
+      <c r="B470">
+        <v>1</v>
+      </c>
+      <c r="C470" t="s">
+        <v>36</v>
+      </c>
+      <c r="D470">
+        <v>-13.557142857142859</v>
+      </c>
+      <c r="E470">
+        <v>33.514285714285712</v>
+      </c>
+      <c r="F470" t="s">
+        <v>12</v>
+      </c>
+      <c r="H470" t="s">
+        <v>120</v>
+      </c>
+      <c r="I470" t="s">
+        <v>79</v>
+      </c>
+      <c r="J470">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="471" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>32</v>
+      </c>
+      <c r="B471">
+        <v>2</v>
+      </c>
+      <c r="C471" t="s">
+        <v>36</v>
+      </c>
+      <c r="D471">
+        <v>-13.3</v>
+      </c>
+      <c r="E471">
+        <v>39.125</v>
+      </c>
+      <c r="F471" t="s">
+        <v>13</v>
+      </c>
+      <c r="H471" t="s">
+        <v>120</v>
+      </c>
+      <c r="I471" t="s">
+        <v>79</v>
+      </c>
+      <c r="J471">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="472" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>18</v>
+      </c>
+      <c r="B472">
+        <v>1</v>
+      </c>
+      <c r="C472" t="s">
+        <v>35</v>
+      </c>
+      <c r="D472">
+        <v>2.3488888888888888</v>
+      </c>
+      <c r="E472">
+        <v>10.31111111111111</v>
+      </c>
+      <c r="F472" t="s">
+        <v>0</v>
+      </c>
+      <c r="H472" t="s">
+        <v>122</v>
+      </c>
+      <c r="I472" t="s">
+        <v>79</v>
+      </c>
+      <c r="J472">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="473" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>18</v>
+      </c>
+      <c r="B473">
+        <v>2</v>
+      </c>
+      <c r="C473" t="s">
+        <v>35</v>
+      </c>
+      <c r="D473">
+        <v>-1.753125</v>
+      </c>
+      <c r="E473">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F473" t="s">
+        <v>1</v>
+      </c>
+      <c r="H473" t="s">
+        <v>122</v>
+      </c>
+      <c r="I473" t="s">
+        <v>79</v>
+      </c>
+      <c r="J473">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="474" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>44</v>
+      </c>
+      <c r="B474">
+        <v>1</v>
+      </c>
+      <c r="C474" t="s">
+        <v>36</v>
+      </c>
+      <c r="D474">
+        <v>-1.753125</v>
+      </c>
+      <c r="E474">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F474" t="s">
+        <v>1</v>
+      </c>
+      <c r="H474" t="s">
+        <v>122</v>
+      </c>
+      <c r="I474" t="s">
+        <v>79</v>
+      </c>
+      <c r="J474">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="475" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>44</v>
+      </c>
+      <c r="B475">
+        <v>2</v>
+      </c>
+      <c r="C475" t="s">
+        <v>36</v>
+      </c>
+      <c r="D475">
+        <v>-0.40769230769230752</v>
+      </c>
+      <c r="E475">
+        <v>21.388461538461538</v>
+      </c>
+      <c r="F475" t="s">
+        <v>2</v>
+      </c>
+      <c r="H475" t="s">
+        <v>122</v>
+      </c>
+      <c r="I475" t="s">
+        <v>79</v>
+      </c>
+      <c r="J475">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="476" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>21</v>
+      </c>
+      <c r="B476">
+        <v>1</v>
+      </c>
+      <c r="C476" t="s">
+        <v>36</v>
+      </c>
+      <c r="D476">
+        <v>-0.40769230769230752</v>
+      </c>
+      <c r="E476">
+        <v>21.388461538461538</v>
+      </c>
+      <c r="F476" t="s">
+        <v>2</v>
+      </c>
+      <c r="H476" t="s">
+        <v>122</v>
+      </c>
+      <c r="I476" t="s">
+        <v>79</v>
+      </c>
+      <c r="J476">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="477" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
+        <v>21</v>
+      </c>
+      <c r="B477">
+        <v>2</v>
+      </c>
+      <c r="C477" t="s">
+        <v>36</v>
+      </c>
+      <c r="D477">
+        <v>-1.78</v>
+      </c>
+      <c r="E477">
+        <v>27.603999999999996</v>
+      </c>
+      <c r="F477" t="s">
+        <v>3</v>
+      </c>
+      <c r="H477" t="s">
+        <v>122</v>
+      </c>
+      <c r="I477" t="s">
+        <v>79</v>
+      </c>
+      <c r="J477">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="478" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>23</v>
+      </c>
+      <c r="B478">
+        <v>1</v>
+      </c>
+      <c r="C478" t="s">
+        <v>35</v>
+      </c>
+      <c r="D478">
+        <v>-1.78</v>
+      </c>
+      <c r="E478">
+        <v>27.603999999999996</v>
+      </c>
+      <c r="F478" t="s">
+        <v>3</v>
+      </c>
+      <c r="H478" t="s">
+        <v>122</v>
+      </c>
+      <c r="I478" t="s">
+        <v>79</v>
+      </c>
+      <c r="J478">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="479" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>23</v>
+      </c>
+      <c r="B479">
+        <v>2</v>
+      </c>
+      <c r="C479" t="s">
+        <v>35</v>
+      </c>
+      <c r="D479">
+        <v>-9.16</v>
+      </c>
+      <c r="E479">
+        <v>26.439999999999998</v>
+      </c>
+      <c r="F479" t="s">
+        <v>10</v>
+      </c>
+      <c r="H479" t="s">
+        <v>122</v>
+      </c>
+      <c r="I479" t="s">
+        <v>79</v>
+      </c>
+      <c r="J479">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="480" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>27</v>
+      </c>
+      <c r="B480">
+        <v>1</v>
+      </c>
+      <c r="C480" t="s">
+        <v>36</v>
+      </c>
+      <c r="D480">
+        <v>-9.16</v>
+      </c>
+      <c r="E480">
+        <v>26.439999999999998</v>
+      </c>
+      <c r="F480" t="s">
+        <v>10</v>
+      </c>
+      <c r="H480" t="s">
+        <v>122</v>
+      </c>
+      <c r="I480" t="s">
+        <v>79</v>
+      </c>
+      <c r="J480">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="481" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>27</v>
+      </c>
+      <c r="B481">
+        <v>2</v>
+      </c>
+      <c r="C481" t="s">
+        <v>36</v>
+      </c>
+      <c r="D481">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E481">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F481" t="s">
+        <v>9</v>
+      </c>
+      <c r="H481" t="s">
+        <v>122</v>
+      </c>
+      <c r="I481" t="s">
+        <v>79</v>
+      </c>
+      <c r="J481">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="482" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>28</v>
+      </c>
+      <c r="B482">
+        <v>1</v>
+      </c>
+      <c r="C482" t="s">
+        <v>35</v>
+      </c>
+      <c r="D482">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E482">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F482" t="s">
+        <v>9</v>
+      </c>
+      <c r="H482" t="s">
+        <v>122</v>
+      </c>
+      <c r="I482" t="s">
+        <v>79</v>
+      </c>
+      <c r="J482">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="483" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
+        <v>28</v>
+      </c>
+      <c r="B483">
+        <v>2</v>
+      </c>
+      <c r="C483" t="s">
+        <v>35</v>
+      </c>
+      <c r="D483">
+        <v>-15.824999999999999</v>
+      </c>
+      <c r="E483">
+        <v>15.45</v>
+      </c>
+      <c r="F483" t="s">
+        <v>14</v>
+      </c>
+      <c r="H483" t="s">
+        <v>122</v>
+      </c>
+      <c r="I483" t="s">
+        <v>79</v>
+      </c>
+      <c r="J483">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="484" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>74</v>
+      </c>
+      <c r="B484">
+        <v>1</v>
+      </c>
+      <c r="C484" t="s">
+        <v>36</v>
+      </c>
+      <c r="D484">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E484">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F484" t="s">
+        <v>9</v>
+      </c>
+      <c r="H484" t="s">
+        <v>122</v>
+      </c>
+      <c r="I484" t="s">
+        <v>79</v>
+      </c>
+      <c r="J484">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="485" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>74</v>
+      </c>
+      <c r="B485">
+        <v>2</v>
+      </c>
+      <c r="C485" t="s">
+        <v>36</v>
+      </c>
+      <c r="D485">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E485">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F485" t="s">
+        <v>11</v>
+      </c>
+      <c r="H485" t="s">
+        <v>122</v>
+      </c>
+      <c r="I485" t="s">
+        <v>79</v>
+      </c>
+      <c r="J485">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="486" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>31</v>
+      </c>
+      <c r="B486">
+        <v>1</v>
+      </c>
+      <c r="C486" t="s">
+        <v>36</v>
+      </c>
+      <c r="D486">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E486">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F486" t="s">
+        <v>11</v>
+      </c>
+      <c r="H486" t="s">
+        <v>122</v>
+      </c>
+      <c r="I486" t="s">
+        <v>79</v>
+      </c>
+      <c r="J486">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="487" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>31</v>
+      </c>
+      <c r="B487">
+        <v>2</v>
+      </c>
+      <c r="C487" t="s">
+        <v>36</v>
+      </c>
+      <c r="D487">
+        <v>-13.557142857142859</v>
+      </c>
+      <c r="E487">
+        <v>33.514285714285712</v>
+      </c>
+      <c r="F487" t="s">
+        <v>12</v>
+      </c>
+      <c r="H487" t="s">
+        <v>122</v>
+      </c>
+      <c r="I487" t="s">
+        <v>79</v>
+      </c>
+      <c r="J487">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="488" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>32</v>
+      </c>
+      <c r="B488">
+        <v>1</v>
+      </c>
+      <c r="C488" t="s">
+        <v>36</v>
+      </c>
+      <c r="D488">
+        <v>-13.557142857142859</v>
+      </c>
+      <c r="E488">
+        <v>33.514285714285712</v>
+      </c>
+      <c r="F488" t="s">
+        <v>12</v>
+      </c>
+      <c r="H488" t="s">
+        <v>122</v>
+      </c>
+      <c r="I488" t="s">
+        <v>79</v>
+      </c>
+      <c r="J488">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="489" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
+        <v>32</v>
+      </c>
+      <c r="B489">
+        <v>2</v>
+      </c>
+      <c r="C489" t="s">
+        <v>36</v>
+      </c>
+      <c r="D489">
+        <v>-13.3</v>
+      </c>
+      <c r="E489">
+        <v>39.125</v>
+      </c>
+      <c r="F489" t="s">
+        <v>13</v>
+      </c>
+      <c r="H489" t="s">
+        <v>122</v>
+      </c>
+      <c r="I489" t="s">
+        <v>79</v>
+      </c>
+      <c r="J489">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="490" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A490" t="s">
+        <v>30</v>
+      </c>
+      <c r="B490">
+        <v>1</v>
+      </c>
+      <c r="C490" t="s">
+        <v>35</v>
+      </c>
+      <c r="D490">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E490">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F490" t="s">
+        <v>11</v>
+      </c>
+      <c r="H490" t="s">
+        <v>122</v>
+      </c>
+      <c r="I490" t="s">
+        <v>79</v>
+      </c>
+      <c r="J490">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="491" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>30</v>
+      </c>
+      <c r="B491">
+        <v>2</v>
+      </c>
+      <c r="C491" t="s">
+        <v>35</v>
+      </c>
+      <c r="D491">
+        <v>-23.125</v>
+      </c>
+      <c r="E491">
+        <v>29.665624999999999</v>
+      </c>
+      <c r="F491" t="s">
+        <v>15</v>
+      </c>
+      <c r="H491" t="s">
+        <v>122</v>
+      </c>
+      <c r="I491" t="s">
+        <v>79</v>
+      </c>
+      <c r="J491">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="492" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>22</v>
+      </c>
+      <c r="B492">
+        <v>1</v>
+      </c>
+      <c r="C492" t="s">
+        <v>35</v>
+      </c>
+      <c r="D492">
+        <v>-1.78</v>
+      </c>
+      <c r="E492">
+        <v>27.603999999999996</v>
+      </c>
+      <c r="F492" t="s">
+        <v>3</v>
+      </c>
+      <c r="H492" t="s">
+        <v>122</v>
+      </c>
+      <c r="I492" t="s">
+        <v>79</v>
+      </c>
+      <c r="J492">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="493" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>22</v>
+      </c>
+      <c r="B493">
+        <v>2</v>
+      </c>
+      <c r="C493" t="s">
+        <v>35</v>
+      </c>
+      <c r="D493">
+        <v>-1.44444444444444</v>
+      </c>
+      <c r="E493">
+        <v>30.911111111111115</v>
+      </c>
+      <c r="F493" t="s">
+        <v>8</v>
+      </c>
+      <c r="H493" t="s">
+        <v>122</v>
+      </c>
+      <c r="I493" t="s">
+        <v>79</v>
+      </c>
+      <c r="J493">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="494" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A494" t="s">
+        <v>24</v>
+      </c>
+      <c r="B494">
+        <v>1</v>
+      </c>
+      <c r="C494" t="s">
+        <v>36</v>
+      </c>
+      <c r="D494">
+        <v>-1.44444444444444</v>
+      </c>
+      <c r="E494">
+        <v>30.911111111111115</v>
+      </c>
+      <c r="F494" t="s">
+        <v>8</v>
+      </c>
+      <c r="H494" t="s">
+        <v>122</v>
+      </c>
+      <c r="I494" t="s">
+        <v>79</v>
+      </c>
+      <c r="J494">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="495" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>24</v>
+      </c>
+      <c r="B495">
+        <v>2</v>
+      </c>
+      <c r="C495" t="s">
+        <v>36</v>
+      </c>
+      <c r="D495">
+        <v>-3.7333333333333329</v>
+      </c>
+      <c r="E495">
+        <v>33</v>
+      </c>
+      <c r="F495" t="s">
+        <v>5</v>
+      </c>
+      <c r="H495" t="s">
+        <v>122</v>
+      </c>
+      <c r="I495" t="s">
+        <v>79</v>
+      </c>
+      <c r="J495">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="496" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>25</v>
+      </c>
+      <c r="B496">
+        <v>1</v>
+      </c>
+      <c r="C496" t="s">
+        <v>36</v>
+      </c>
+      <c r="D496">
+        <v>-3.7333333333333329</v>
+      </c>
+      <c r="E496">
+        <v>33</v>
+      </c>
+      <c r="F496" t="s">
+        <v>5</v>
+      </c>
+      <c r="H496" t="s">
+        <v>122</v>
+      </c>
+      <c r="I496" t="s">
+        <v>79</v>
+      </c>
+      <c r="J496">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="497" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>25</v>
+      </c>
+      <c r="B497">
+        <v>2</v>
+      </c>
+      <c r="C497" t="s">
+        <v>36</v>
+      </c>
+      <c r="D497">
+        <v>-5.85</v>
+      </c>
+      <c r="E497">
+        <v>37.712499999999999</v>
+      </c>
+      <c r="F497" t="s">
+        <v>6</v>
+      </c>
+      <c r="H497" t="s">
+        <v>122</v>
+      </c>
+      <c r="I497" t="s">
+        <v>79</v>
+      </c>
+      <c r="J497">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="498" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
+        <v>26</v>
+      </c>
+      <c r="B498">
+        <v>1</v>
+      </c>
+      <c r="C498" t="s">
+        <v>35</v>
+      </c>
+      <c r="D498">
+        <v>-5.85</v>
+      </c>
+      <c r="E498">
+        <v>37.712499999999999</v>
+      </c>
+      <c r="F498" t="s">
+        <v>6</v>
+      </c>
+      <c r="H498" t="s">
+        <v>122</v>
+      </c>
+      <c r="I498" t="s">
+        <v>79</v>
+      </c>
+      <c r="J498">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="499" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
+        <v>26</v>
+      </c>
+      <c r="B499">
+        <v>2</v>
+      </c>
+      <c r="C499" t="s">
+        <v>35</v>
+      </c>
+      <c r="D499">
+        <v>-2.35</v>
+      </c>
+      <c r="E499">
+        <v>38.449999999999996</v>
+      </c>
+      <c r="F499" t="s">
+        <v>4</v>
+      </c>
+      <c r="H499" t="s">
+        <v>122</v>
+      </c>
+      <c r="I499" t="s">
+        <v>79</v>
+      </c>
+      <c r="J499">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="500" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>19</v>
+      </c>
+      <c r="B500">
+        <v>1</v>
+      </c>
+      <c r="C500" t="s">
+        <v>35</v>
+      </c>
+      <c r="D500">
+        <v>-1.753125</v>
+      </c>
+      <c r="E500">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F500" t="s">
+        <v>1</v>
+      </c>
+      <c r="H500" t="s">
+        <v>122</v>
+      </c>
+      <c r="I500" t="s">
+        <v>79</v>
+      </c>
+      <c r="J500">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="501" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A501" t="s">
+        <v>19</v>
+      </c>
+      <c r="B501">
+        <v>2</v>
+      </c>
+      <c r="C501" t="s">
+        <v>35</v>
+      </c>
+      <c r="D501">
+        <v>-5.5714285714285703</v>
+      </c>
+      <c r="E501">
+        <v>15.75</v>
+      </c>
+      <c r="F501" t="s">
+        <v>7</v>
+      </c>
+      <c r="H501" t="s">
+        <v>122</v>
+      </c>
+      <c r="I501" t="s">
+        <v>79</v>
+      </c>
+      <c r="J501">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J381" xr:uid="{303E4824-0DA0-4156-A165-CC92066081A2}"/>
+  <autoFilter ref="A1:J501" xr:uid="{303E4824-0DA0-4156-A165-CC92066081A2}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add model grid for all 5 models (AMNH), Rename latest AMNH models
</commit_message>
<xml_diff>
--- a/resources/datasets/MigratoryModel/CombinedMigratoryModel_GuthrieZone_Path - AllModels.xlsx
+++ b/resources/datasets/MigratoryModel/CombinedMigratoryModel_GuthrieZone_Path - AllModels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby Ford\Desktop\BantuMigration\Github\resources\datasets\MigratoryModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD91C202-3064-4B34-A289-8C5267BE303E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2E8054-CB6C-467E-91F3-3DB311736C05}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48220AAF-5FA7-46D3-8056-2130CE6EF7AB}"/>
   </bookViews>
@@ -391,13 +391,13 @@
     <t>AMNH - Combined 400 -11-H</t>
   </si>
   <si>
-    <t>new-jan_lang-sw-11-H</t>
-  </si>
-  <si>
     <t>N-M</t>
   </si>
   <si>
-    <t>new-jan_lang-sw-all5-H</t>
+    <t>AMNH - Language (sw-11-H)</t>
+  </si>
+  <si>
+    <t>AMNH - Language (sw-all5-H)</t>
   </si>
 </sst>
 </file>
@@ -752,7 +752,7 @@
   <dimension ref="A1:J501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F455" sqref="F455"/>
+      <selection activeCell="H472" sqref="H472:H501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14211,7 +14211,7 @@
         <v>0</v>
       </c>
       <c r="H442" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I442" t="s">
         <v>79</v>
@@ -14240,7 +14240,7 @@
         <v>1</v>
       </c>
       <c r="H443" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I443" t="s">
         <v>79</v>
@@ -14269,7 +14269,7 @@
         <v>1</v>
       </c>
       <c r="H444" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I444" t="s">
         <v>79</v>
@@ -14298,7 +14298,7 @@
         <v>7</v>
       </c>
       <c r="H445" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I445" t="s">
         <v>79</v>
@@ -14327,7 +14327,7 @@
         <v>1</v>
       </c>
       <c r="H446" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I446" t="s">
         <v>79</v>
@@ -14356,7 +14356,7 @@
         <v>2</v>
       </c>
       <c r="H447" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I447" t="s">
         <v>79</v>
@@ -14385,7 +14385,7 @@
         <v>2</v>
       </c>
       <c r="H448" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I448" t="s">
         <v>79</v>
@@ -14414,7 +14414,7 @@
         <v>3</v>
       </c>
       <c r="H449" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I449" t="s">
         <v>79</v>
@@ -14443,7 +14443,7 @@
         <v>3</v>
       </c>
       <c r="H450" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I450" t="s">
         <v>79</v>
@@ -14472,7 +14472,7 @@
         <v>8</v>
       </c>
       <c r="H451" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I451" t="s">
         <v>79</v>
@@ -14501,7 +14501,7 @@
         <v>8</v>
       </c>
       <c r="H452" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I452" t="s">
         <v>79</v>
@@ -14530,7 +14530,7 @@
         <v>5</v>
       </c>
       <c r="H453" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I453" t="s">
         <v>79</v>
@@ -14559,7 +14559,7 @@
         <v>5</v>
       </c>
       <c r="H454" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I454" t="s">
         <v>79</v>
@@ -14588,7 +14588,7 @@
         <v>6</v>
       </c>
       <c r="H455" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I455" t="s">
         <v>79</v>
@@ -14617,7 +14617,7 @@
         <v>6</v>
       </c>
       <c r="H456" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I456" t="s">
         <v>79</v>
@@ -14646,7 +14646,7 @@
         <v>4</v>
       </c>
       <c r="H457" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I457" t="s">
         <v>79</v>
@@ -14675,7 +14675,7 @@
         <v>6</v>
       </c>
       <c r="H458" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I458" t="s">
         <v>79</v>
@@ -14704,7 +14704,7 @@
         <v>12</v>
       </c>
       <c r="H459" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I459" t="s">
         <v>79</v>
@@ -14715,7 +14715,7 @@
     </row>
     <row r="460" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B460">
         <v>1</v>
@@ -14733,7 +14733,7 @@
         <v>12</v>
       </c>
       <c r="H460" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I460" t="s">
         <v>79</v>
@@ -14744,7 +14744,7 @@
     </row>
     <row r="461" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B461">
         <v>2</v>
@@ -14762,7 +14762,7 @@
         <v>11</v>
       </c>
       <c r="H461" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I461" t="s">
         <v>79</v>
@@ -14791,7 +14791,7 @@
         <v>11</v>
       </c>
       <c r="H462" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I462" t="s">
         <v>79</v>
@@ -14820,7 +14820,7 @@
         <v>10</v>
       </c>
       <c r="H463" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I463" t="s">
         <v>79</v>
@@ -14849,7 +14849,7 @@
         <v>10</v>
       </c>
       <c r="H464" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I464" t="s">
         <v>79</v>
@@ -14878,7 +14878,7 @@
         <v>9</v>
       </c>
       <c r="H465" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I465" t="s">
         <v>79</v>
@@ -14907,7 +14907,7 @@
         <v>9</v>
       </c>
       <c r="H466" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I466" t="s">
         <v>79</v>
@@ -14936,7 +14936,7 @@
         <v>14</v>
       </c>
       <c r="H467" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I467" t="s">
         <v>79</v>
@@ -14965,7 +14965,7 @@
         <v>11</v>
       </c>
       <c r="H468" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I468" t="s">
         <v>79</v>
@@ -14994,7 +14994,7 @@
         <v>15</v>
       </c>
       <c r="H469" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I469" t="s">
         <v>79</v>
@@ -15023,7 +15023,7 @@
         <v>12</v>
       </c>
       <c r="H470" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I470" t="s">
         <v>79</v>
@@ -15052,7 +15052,7 @@
         <v>13</v>
       </c>
       <c r="H471" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I471" t="s">
         <v>79</v>

</xml_diff>